<commit_message>
Tweaks to dashboard color scheme, alignment, and then deployed.
</commit_message>
<xml_diff>
--- a/dashboard/data/watchdb.all_tables.xlsx
+++ b/dashboard/data/watchdb.all_tables.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/dashboard/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65177306-A7B6-3C48-BF95-C3622DB65A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F12CEAD-B619-CF48-90B2-DBE19C445B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
@@ -2563,7 +2563,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4250,8 +4250,8 @@
       <c r="C30" s="29" t="s">
         <v>359</v>
       </c>
-      <c r="D30" s="32" t="s">
-        <v>103</v>
+      <c r="D30" s="35" t="s">
+        <v>60</v>
       </c>
       <c r="E30" s="29" t="s">
         <v>160</v>

</xml_diff>

<commit_message>
Fixed inconsistency in RSV labels. Removed CheatLake data temporarily bc causing some weird NA bug in the SARS data.
</commit_message>
<xml_diff>
--- a/dashboard/data/watchdb.all_tables.xlsx
+++ b/dashboard/data/watchdb.all_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8F38D1-F561-F04F-A93F-65C1FFF0D50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C47EBFE-D508-5144-B61A-D267D50F7647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="5" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1568" uniqueCount="649">
   <si>
     <t>CharlestonWWTP-01</t>
   </si>
@@ -1847,139 +1847,145 @@
     <t>Ec</t>
   </si>
   <si>
+    <t>Lg</t>
+  </si>
+  <si>
+    <t>Salmonella Enteritidis</t>
+  </si>
+  <si>
+    <t>Salmonella Newport</t>
+  </si>
+  <si>
+    <t>Salmonella Typhimurium</t>
+  </si>
+  <si>
+    <t>Salmonella Javiana</t>
+  </si>
+  <si>
+    <t>Legionairre's Disease</t>
+  </si>
+  <si>
+    <t>16S</t>
+  </si>
+  <si>
+    <t>23S</t>
+  </si>
+  <si>
+    <t>C3b</t>
+  </si>
+  <si>
+    <t>N1:SARS</t>
+  </si>
+  <si>
+    <t>N2:SARS</t>
+  </si>
+  <si>
+    <t>NEP/NS1</t>
+  </si>
+  <si>
+    <t>POL</t>
+  </si>
+  <si>
+    <t>RNase P</t>
+  </si>
+  <si>
+    <t>S:E484K</t>
+  </si>
+  <si>
+    <t>S:E484K WT</t>
+  </si>
+  <si>
+    <t>S:HVdel69-70</t>
+  </si>
+  <si>
+    <t>S:HVdel69-70 WT</t>
+  </si>
+  <si>
+    <t>S:N501Y</t>
+  </si>
+  <si>
+    <t>S:N501Y WT</t>
+  </si>
+  <si>
+    <t>TNFR</t>
+  </si>
+  <si>
+    <t>locus_id</t>
+  </si>
+  <si>
+    <t>SaltRock WWTP: Ona and SaltRock</t>
+  </si>
+  <si>
+    <t>SaltRock WWTP: Milton and Culloden</t>
+  </si>
+  <si>
+    <t>CharlestonWVU</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>Hometown-Putnam</t>
+  </si>
+  <si>
+    <t>PutnamPSD</t>
+  </si>
+  <si>
+    <t>3rdAndHalGreerMU</t>
+  </si>
+  <si>
+    <t>CommonsDormsMU</t>
+  </si>
+  <si>
+    <t>SRCM</t>
+  </si>
+  <si>
+    <t>TwinTowersEastDormMU</t>
+  </si>
+  <si>
+    <t>TwinTowersWestDormMU</t>
+  </si>
+  <si>
+    <t>MU HACH</t>
+  </si>
+  <si>
+    <t>Manhole collects from Willis, Gibson, and Wellman dormatories - Haymaker WW goes toward Harless Cafe</t>
+  </si>
+  <si>
+    <t>Manhole located on the corner of 3rd Avene and Hal Greer. Collects from parts or all of Smith Music Hall, Smith Hall, Communications Building, and Science Building, Morrow, and Old Main</t>
+  </si>
+  <si>
+    <t>Lagoon - plan to pump into PeaRidge some day when new pearidge plant comes to be</t>
+  </si>
+  <si>
+    <t>Upstream from Huntington Sanitary board</t>
+  </si>
+  <si>
+    <t>Small independent plant under PeaRidge management</t>
+  </si>
+  <si>
+    <t>HometownWWTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 54079-002-01-00-00</t>
+  </si>
+  <si>
+    <t>Putnam PSD</t>
+  </si>
+  <si>
+    <t>WV0028045</t>
+  </si>
+  <si>
+    <t>M:FLUA</t>
+  </si>
+  <si>
+    <t>SC2:SARS</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
     <t>Human</t>
-  </si>
-  <si>
-    <t>Lg</t>
-  </si>
-  <si>
-    <t>Salmonella Enteritidis</t>
-  </si>
-  <si>
-    <t>Salmonella Newport</t>
-  </si>
-  <si>
-    <t>Salmonella Typhimurium</t>
-  </si>
-  <si>
-    <t>Salmonella Javiana</t>
-  </si>
-  <si>
-    <t>Legionairre's Disease</t>
-  </si>
-  <si>
-    <t>16S</t>
-  </si>
-  <si>
-    <t>23S</t>
-  </si>
-  <si>
-    <t>C3b</t>
-  </si>
-  <si>
-    <t>N1:SARS</t>
-  </si>
-  <si>
-    <t>N2:SARS</t>
-  </si>
-  <si>
-    <t>NEP/NS1</t>
-  </si>
-  <si>
-    <t>POL</t>
-  </si>
-  <si>
-    <t>RNase P</t>
-  </si>
-  <si>
-    <t>S:E484K</t>
-  </si>
-  <si>
-    <t>S:E484K WT</t>
-  </si>
-  <si>
-    <t>S:HVdel69-70</t>
-  </si>
-  <si>
-    <t>S:HVdel69-70 WT</t>
-  </si>
-  <si>
-    <t>S:N501Y</t>
-  </si>
-  <si>
-    <t>S:N501Y WT</t>
-  </si>
-  <si>
-    <t>TNFR</t>
-  </si>
-  <si>
-    <t>locus_id</t>
-  </si>
-  <si>
-    <t>SaltRock WWTP: Ona and SaltRock</t>
-  </si>
-  <si>
-    <t>SaltRock WWTP: Milton and Culloden</t>
-  </si>
-  <si>
-    <t>CharlestonWVU</t>
-  </si>
-  <si>
-    <t>PUT</t>
-  </si>
-  <si>
-    <t>Hometown-Putnam</t>
-  </si>
-  <si>
-    <t>PutnamPSD</t>
-  </si>
-  <si>
-    <t>3rdAndHalGreerMU</t>
-  </si>
-  <si>
-    <t>CommonsDormsMU</t>
-  </si>
-  <si>
-    <t>SRCM</t>
-  </si>
-  <si>
-    <t>TwinTowersEastDormMU</t>
-  </si>
-  <si>
-    <t>TwinTowersWestDormMU</t>
-  </si>
-  <si>
-    <t>MU HACH</t>
-  </si>
-  <si>
-    <t>Manhole collects from Willis, Gibson, and Wellman dormatories - Haymaker WW goes toward Harless Cafe</t>
-  </si>
-  <si>
-    <t>Manhole located on the corner of 3rd Avene and Hal Greer. Collects from parts or all of Smith Music Hall, Smith Hall, Communications Building, and Science Building, Morrow, and Old Main</t>
-  </si>
-  <si>
-    <t>Lagoon - plan to pump into PeaRidge some day when new pearidge plant comes to be</t>
-  </si>
-  <si>
-    <t>Upstream from Huntington Sanitary board</t>
-  </si>
-  <si>
-    <t>Small independent plant under PeaRidge management</t>
-  </si>
-  <si>
-    <t>HometownWWTP</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 54079-002-01-00-00</t>
-  </si>
-  <si>
-    <t>Putnam PSD</t>
-  </si>
-  <si>
-    <t>WV0028045</t>
-  </si>
-  <si>
-    <t>M:FLUA</t>
   </si>
 </sst>
 </file>
@@ -2623,10 +2629,10 @@
   <dimension ref="A1:T81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O28" sqref="O28"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2784,7 +2790,7 @@
         <v>60</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>340</v>
@@ -2892,8 +2898,8 @@
       <c r="C5" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>103</v>
+      <c r="D5" s="40" t="s">
+        <v>60</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>102</v>
@@ -4080,14 +4086,14 @@
         <v>38.424089000000002</v>
       </c>
       <c r="J25" s="46" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="K25" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L25" s="33"/>
       <c r="M25" s="33" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="N25" s="33">
         <v>5</v>
@@ -4108,7 +4114,7 @@
         <v>25703</v>
       </c>
       <c r="T25" s="46" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="26" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -4147,7 +4153,7 @@
         <v>4000</v>
       </c>
       <c r="M26" s="33" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="N26" s="33">
         <v>24</v>
@@ -4168,7 +4174,7 @@
         <v>25504</v>
       </c>
       <c r="T26" s="47" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="27" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4198,14 +4204,14 @@
         <v>38.421745999999999</v>
       </c>
       <c r="J27" s="46" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="K27" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L27" s="33"/>
       <c r="M27" s="33" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="N27" s="33">
         <v>5</v>
@@ -4226,7 +4232,7 @@
         <v>25703</v>
       </c>
       <c r="T27" s="46" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="28" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4514,7 +4520,7 @@
         <v>25701</v>
       </c>
       <c r="T32" s="29" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
@@ -4574,7 +4580,7 @@
         <v>25537</v>
       </c>
       <c r="T33" s="29" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="34" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -4613,7 +4619,7 @@
         <v>7000</v>
       </c>
       <c r="M34" s="34" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="N34" s="34">
         <v>24</v>
@@ -4637,7 +4643,7 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="29" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B35" s="29"/>
       <c r="C35" s="29" t="s">
@@ -4647,7 +4653,7 @@
         <v>103</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F35" s="29" t="s">
         <v>340</v>
@@ -4707,7 +4713,7 @@
         <v>103</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F36" s="29" t="s">
         <v>340</v>
@@ -4782,14 +4788,14 @@
         <v>38.422913110104098</v>
       </c>
       <c r="J37" s="46" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="K37" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L37" s="33"/>
       <c r="M37" s="34" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="N37" s="33">
         <v>5</v>
@@ -4838,14 +4844,14 @@
         <v>38.423076174075902</v>
       </c>
       <c r="J38" s="46" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="K38" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L38" s="33"/>
       <c r="M38" s="34" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="N38" s="33">
         <v>24</v>
@@ -4869,7 +4875,7 @@
     </row>
     <row r="39" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="46" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B39" s="46"/>
       <c r="C39" s="46" t="s">
@@ -4879,7 +4885,7 @@
         <v>103</v>
       </c>
       <c r="E39" s="46" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F39" s="46" t="s">
         <v>340</v>
@@ -4894,7 +4900,7 @@
         <v>38.537901317549398</v>
       </c>
       <c r="J39" s="46" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="K39" s="46" t="s">
         <v>159</v>
@@ -8594,22 +8600,22 @@
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="51" t="s">
+        <v>641</v>
+      </c>
+      <c r="B47" s="52" t="s">
         <v>642</v>
       </c>
-      <c r="B47" s="52" t="s">
+      <c r="C47" s="51" t="s">
+        <v>628</v>
+      </c>
+      <c r="D47" s="51" t="s">
         <v>643</v>
-      </c>
-      <c r="C47" s="51" t="s">
-        <v>629</v>
-      </c>
-      <c r="D47" s="51" t="s">
-        <v>644</v>
       </c>
       <c r="E47" s="51" t="s">
         <v>159</v>
       </c>
       <c r="F47" s="51" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G47" s="51"/>
       <c r="H47" s="51">
@@ -9679,9 +9685,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274C28A9-51BA-1349-BC2C-74CFA9B6CA14}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9889,7 +9895,7 @@
         <v>590</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>417</v>
@@ -9898,7 +9904,7 @@
         <v>382</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="19" x14ac:dyDescent="0.25">
@@ -10048,7 +10054,7 @@
         <v>594</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C19" s="25" t="s">
         <v>417</v>
@@ -10065,7 +10071,7 @@
         <v>595</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C20" s="25" t="s">
         <v>417</v>
@@ -10082,7 +10088,7 @@
         <v>596</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C21" s="25" t="s">
         <v>417</v>
@@ -10099,7 +10105,7 @@
         <v>597</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C22" s="25" t="s">
         <v>417</v>
@@ -10217,15 +10223,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{874AFBB5-8FFB-B248-A4C3-9A81309B9614}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" style="25" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="25"/>
   </cols>
@@ -10235,87 +10241,87 @@
         <v>374</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>586</v>
-      </c>
-      <c r="B2" s="44" t="s">
-        <v>610</v>
+      <c r="A2" s="43" t="s">
+        <v>592</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>647</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>602</v>
+        <v>586</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
-        <v>383</v>
+      <c r="A4" s="25" t="s">
+        <v>648</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>646</v>
+        <v>615</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="45" t="s">
+        <v>383</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="45" t="s">
         <v>386</v>
       </c>
-      <c r="B5" s="44" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="B6" s="44" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
         <v>590</v>
       </c>
-      <c r="B6" s="44" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
-        <v>599</v>
-      </c>
       <c r="B7" s="44" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="45" t="s">
+        <v>599</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="45" t="s">
         <v>600</v>
       </c>
-      <c r="B8" s="44" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
-        <v>389</v>
-      </c>
       <c r="B9" s="44" t="s">
-        <v>615</v>
+        <v>622</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B10" s="44" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="43" t="s">
+        <v>593</v>
+      </c>
+      <c r="B11" s="44" t="s">
         <v>323</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
-        <v>393</v>
-      </c>
-      <c r="B11" s="44" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -10323,7 +10329,7 @@
         <v>393</v>
       </c>
       <c r="B12" s="44" t="s">
-        <v>612</v>
+        <v>321</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -10331,7 +10337,7 @@
         <v>393</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -10339,7 +10345,7 @@
         <v>393</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>335</v>
+        <v>612</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -10347,7 +10353,7 @@
         <v>393</v>
       </c>
       <c r="B15" s="44" t="s">
-        <v>617</v>
+        <v>335</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -10355,7 +10361,7 @@
         <v>393</v>
       </c>
       <c r="B16" s="44" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -10363,7 +10369,7 @@
         <v>393</v>
       </c>
       <c r="B17" s="44" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -10371,7 +10377,7 @@
         <v>393</v>
       </c>
       <c r="B18" s="44" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -10379,7 +10385,7 @@
         <v>393</v>
       </c>
       <c r="B19" s="44" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -10387,15 +10393,28 @@
         <v>393</v>
       </c>
       <c r="B20" s="44" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="44"/>
+      <c r="A21" s="25" t="s">
+        <v>393</v>
+      </c>
+      <c r="B21" s="44" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
+        <v>393</v>
+      </c>
+      <c r="B22" s="44" t="s">
+        <v>646</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B20">
-    <sortCondition ref="A2:A20"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B21">
+    <sortCondition ref="A3:A21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Data update. West Union and CL not behaving - some sort of format issue maybe? - so they are inactivated for now.
</commit_message>
<xml_diff>
--- a/dashboard/data/watchdb.all_tables.xlsx
+++ b/dashboard/data/watchdb.all_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C47EBFE-D508-5144-B61A-D267D50F7647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BC44EC-1990-FC42-A72F-CAD8519FF0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1568" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="647">
   <si>
     <t>CharlestonWWTP-01</t>
   </si>
@@ -1977,12 +1977,6 @@
   </si>
   <si>
     <t>M:FLUA</t>
-  </si>
-  <si>
-    <t>SC2:SARS</t>
-  </si>
-  <si>
-    <t>Other</t>
   </si>
   <si>
     <t>Human</t>
@@ -1995,7 +1989,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2141,8 +2135,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2173,6 +2174,12 @@
         <bgColor rgb="FFE2EFD9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2187,7 +2194,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2304,6 +2311,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2628,11 +2638,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0856F7A-D0C0-3942-9027-9FB2F3C2C3E0}">
   <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2898,7 +2908,7 @@
       <c r="C5" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="54" t="s">
         <v>60</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -3894,8 +3904,8 @@
       <c r="C22" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>103</v>
+      <c r="D22" s="54" t="s">
+        <v>60</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>84</v>
@@ -9685,9 +9695,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274C28A9-51BA-1349-BC2C-74CFA9B6CA14}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10223,15 +10233,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{874AFBB5-8FFB-B248-A4C3-9A81309B9614}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.5" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" style="25" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="25"/>
   </cols>
@@ -10245,83 +10255,83 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
-        <v>592</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>647</v>
+      <c r="A2" s="25" t="s">
+        <v>586</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>609</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>586</v>
+        <v>646</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>609</v>
+        <v>615</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
-        <v>648</v>
+      <c r="A4" s="45" t="s">
+        <v>383</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>615</v>
+        <v>645</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="45" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>645</v>
+        <v>613</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
-        <v>386</v>
+      <c r="A6" s="25" t="s">
+        <v>590</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
-        <v>590</v>
+      <c r="A7" s="45" t="s">
+        <v>599</v>
       </c>
       <c r="B7" s="44" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="45" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B8" s="44" t="s">
-        <v>610</v>
+        <v>622</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="45" t="s">
-        <v>600</v>
+      <c r="A9" s="25" t="s">
+        <v>389</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>622</v>
+        <v>614</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>614</v>
+        <v>323</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
-        <v>593</v>
+      <c r="A11" s="25" t="s">
+        <v>393</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -10329,7 +10339,7 @@
         <v>393</v>
       </c>
       <c r="B12" s="44" t="s">
-        <v>321</v>
+        <v>611</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -10337,7 +10347,7 @@
         <v>393</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -10345,7 +10355,7 @@
         <v>393</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>612</v>
+        <v>335</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -10353,7 +10363,7 @@
         <v>393</v>
       </c>
       <c r="B15" s="44" t="s">
-        <v>335</v>
+        <v>616</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -10361,7 +10371,7 @@
         <v>393</v>
       </c>
       <c r="B16" s="44" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -10369,7 +10379,7 @@
         <v>393</v>
       </c>
       <c r="B17" s="44" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -10377,7 +10387,7 @@
         <v>393</v>
       </c>
       <c r="B18" s="44" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -10385,7 +10395,7 @@
         <v>393</v>
       </c>
       <c r="B19" s="44" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -10393,28 +10403,15 @@
         <v>393</v>
       </c>
       <c r="B20" s="44" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
-        <v>393</v>
-      </c>
-      <c r="B21" s="44" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
-        <v>393</v>
-      </c>
-      <c r="B22" s="44" t="s">
-        <v>646</v>
-      </c>
+      <c r="B21" s="44"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B21">
-    <sortCondition ref="A3:A21"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B20">
+    <sortCondition ref="A2:A20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Removal of 1st quarter data to data depot.
</commit_message>
<xml_diff>
--- a/dashboard/data/watchdb.all_tables.xlsx
+++ b/dashboard/data/watchdb.all_tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/dashboard/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BC44EC-1990-FC42-A72F-CAD8519FF0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B72292-9838-BA47-8870-E3972E546152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="5" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="647">
   <si>
     <t>CharlestonWWTP-01</t>
   </si>
@@ -1874,112 +1874,112 @@
     <t>C3b</t>
   </si>
   <si>
-    <t>N1:SARS</t>
-  </si>
-  <si>
-    <t>N2:SARS</t>
+    <t>POL</t>
+  </si>
+  <si>
+    <t>RNase P</t>
+  </si>
+  <si>
+    <t>S:E484K</t>
+  </si>
+  <si>
+    <t>S:E484K WT</t>
+  </si>
+  <si>
+    <t>S:HVdel69-70</t>
+  </si>
+  <si>
+    <t>S:HVdel69-70 WT</t>
+  </si>
+  <si>
+    <t>S:N501Y</t>
+  </si>
+  <si>
+    <t>S:N501Y WT</t>
+  </si>
+  <si>
+    <t>TNFR</t>
+  </si>
+  <si>
+    <t>locus_id</t>
+  </si>
+  <si>
+    <t>SaltRock WWTP: Ona and SaltRock</t>
+  </si>
+  <si>
+    <t>SaltRock WWTP: Milton and Culloden</t>
+  </si>
+  <si>
+    <t>CharlestonWVU</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>Hometown-Putnam</t>
+  </si>
+  <si>
+    <t>PutnamPSD</t>
+  </si>
+  <si>
+    <t>3rdAndHalGreerMU</t>
+  </si>
+  <si>
+    <t>CommonsDormsMU</t>
+  </si>
+  <si>
+    <t>SRCM</t>
+  </si>
+  <si>
+    <t>TwinTowersEastDormMU</t>
+  </si>
+  <si>
+    <t>TwinTowersWestDormMU</t>
+  </si>
+  <si>
+    <t>MU HACH</t>
+  </si>
+  <si>
+    <t>Manhole collects from Willis, Gibson, and Wellman dormatories - Haymaker WW goes toward Harless Cafe</t>
+  </si>
+  <si>
+    <t>Manhole located on the corner of 3rd Avene and Hal Greer. Collects from parts or all of Smith Music Hall, Smith Hall, Communications Building, and Science Building, Morrow, and Old Main</t>
+  </si>
+  <si>
+    <t>Lagoon - plan to pump into PeaRidge some day when new pearidge plant comes to be</t>
+  </si>
+  <si>
+    <t>Upstream from Huntington Sanitary board</t>
+  </si>
+  <si>
+    <t>Small independent plant under PeaRidge management</t>
+  </si>
+  <si>
+    <t>HometownWWTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 54079-002-01-00-00</t>
+  </si>
+  <si>
+    <t>Putnam PSD</t>
+  </si>
+  <si>
+    <t>WV0028045</t>
+  </si>
+  <si>
+    <t>Human</t>
   </si>
   <si>
     <t>NEP/NS1</t>
   </si>
   <si>
-    <t>POL</t>
-  </si>
-  <si>
-    <t>RNase P</t>
-  </si>
-  <si>
-    <t>S:E484K</t>
-  </si>
-  <si>
-    <t>S:E484K WT</t>
-  </si>
-  <si>
-    <t>S:HVdel69-70</t>
-  </si>
-  <si>
-    <t>S:HVdel69-70 WT</t>
-  </si>
-  <si>
-    <t>S:N501Y</t>
-  </si>
-  <si>
-    <t>S:N501Y WT</t>
-  </si>
-  <si>
-    <t>TNFR</t>
-  </si>
-  <si>
-    <t>locus_id</t>
-  </si>
-  <si>
-    <t>SaltRock WWTP: Ona and SaltRock</t>
-  </si>
-  <si>
-    <t>SaltRock WWTP: Milton and Culloden</t>
-  </si>
-  <si>
-    <t>CharlestonWVU</t>
-  </si>
-  <si>
-    <t>PUT</t>
-  </si>
-  <si>
-    <t>Hometown-Putnam</t>
-  </si>
-  <si>
-    <t>PutnamPSD</t>
-  </si>
-  <si>
-    <t>3rdAndHalGreerMU</t>
-  </si>
-  <si>
-    <t>CommonsDormsMU</t>
-  </si>
-  <si>
-    <t>SRCM</t>
-  </si>
-  <si>
-    <t>TwinTowersEastDormMU</t>
-  </si>
-  <si>
-    <t>TwinTowersWestDormMU</t>
-  </si>
-  <si>
-    <t>MU HACH</t>
-  </si>
-  <si>
-    <t>Manhole collects from Willis, Gibson, and Wellman dormatories - Haymaker WW goes toward Harless Cafe</t>
-  </si>
-  <si>
-    <t>Manhole located on the corner of 3rd Avene and Hal Greer. Collects from parts or all of Smith Music Hall, Smith Hall, Communications Building, and Science Building, Morrow, and Old Main</t>
-  </si>
-  <si>
-    <t>Lagoon - plan to pump into PeaRidge some day when new pearidge plant comes to be</t>
-  </si>
-  <si>
-    <t>Upstream from Huntington Sanitary board</t>
-  </si>
-  <si>
-    <t>Small independent plant under PeaRidge management</t>
-  </si>
-  <si>
-    <t>HometownWWTP</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 54079-002-01-00-00</t>
-  </si>
-  <si>
-    <t>Putnam PSD</t>
-  </si>
-  <si>
-    <t>WV0028045</t>
-  </si>
-  <si>
-    <t>M:FLUA</t>
-  </si>
-  <si>
-    <t>Human</t>
+    <t>N1</t>
+  </si>
+  <si>
+    <t>N2</t>
+  </si>
+  <si>
+    <t>SC2</t>
   </si>
 </sst>
 </file>
@@ -1989,7 +1989,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2135,15 +2135,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2174,12 +2167,6 @@
         <bgColor rgb="FFE2EFD9"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2194,7 +2181,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2311,9 +2298,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2638,11 +2622,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0856F7A-D0C0-3942-9027-9FB2F3C2C3E0}">
   <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomRight" activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2800,7 +2784,7 @@
         <v>60</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>340</v>
@@ -2908,8 +2892,8 @@
       <c r="C5" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="D5" s="54" t="s">
-        <v>60</v>
+      <c r="D5" s="4" t="s">
+        <v>103</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>102</v>
@@ -3904,8 +3888,8 @@
       <c r="C22" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="D22" s="54" t="s">
-        <v>60</v>
+      <c r="D22" s="4" t="s">
+        <v>103</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>84</v>
@@ -4096,14 +4080,14 @@
         <v>38.424089000000002</v>
       </c>
       <c r="J25" s="46" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="K25" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L25" s="33"/>
       <c r="M25" s="33" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="N25" s="33">
         <v>5</v>
@@ -4124,7 +4108,7 @@
         <v>25703</v>
       </c>
       <c r="T25" s="46" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
     </row>
     <row r="26" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -4163,7 +4147,7 @@
         <v>4000</v>
       </c>
       <c r="M26" s="33" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="N26" s="33">
         <v>24</v>
@@ -4184,7 +4168,7 @@
         <v>25504</v>
       </c>
       <c r="T26" s="47" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
     </row>
     <row r="27" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4214,14 +4198,14 @@
         <v>38.421745999999999</v>
       </c>
       <c r="J27" s="46" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="K27" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L27" s="33"/>
       <c r="M27" s="33" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="N27" s="33">
         <v>5</v>
@@ -4242,7 +4226,7 @@
         <v>25703</v>
       </c>
       <c r="T27" s="46" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
     </row>
     <row r="28" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4530,7 +4514,7 @@
         <v>25701</v>
       </c>
       <c r="T32" s="29" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
@@ -4590,7 +4574,7 @@
         <v>25537</v>
       </c>
       <c r="T33" s="29" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
     </row>
     <row r="34" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -4629,7 +4613,7 @@
         <v>7000</v>
       </c>
       <c r="M34" s="34" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="N34" s="34">
         <v>24</v>
@@ -4653,7 +4637,7 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="29" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="B35" s="29"/>
       <c r="C35" s="29" t="s">
@@ -4663,7 +4647,7 @@
         <v>103</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="F35" s="29" t="s">
         <v>340</v>
@@ -4723,7 +4707,7 @@
         <v>103</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="F36" s="29" t="s">
         <v>340</v>
@@ -4798,14 +4782,14 @@
         <v>38.422913110104098</v>
       </c>
       <c r="J37" s="46" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="K37" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L37" s="33"/>
       <c r="M37" s="34" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="N37" s="33">
         <v>5</v>
@@ -4854,14 +4838,14 @@
         <v>38.423076174075902</v>
       </c>
       <c r="J38" s="46" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="K38" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L38" s="33"/>
       <c r="M38" s="34" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="N38" s="33">
         <v>24</v>
@@ -4885,7 +4869,7 @@
     </row>
     <row r="39" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="46" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="B39" s="46"/>
       <c r="C39" s="46" t="s">
@@ -4895,7 +4879,7 @@
         <v>103</v>
       </c>
       <c r="E39" s="46" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="F39" s="46" t="s">
         <v>340</v>
@@ -4910,7 +4894,7 @@
         <v>38.537901317549398</v>
       </c>
       <c r="J39" s="46" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="K39" s="46" t="s">
         <v>159</v>
@@ -8610,22 +8594,22 @@
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="51" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B47" s="52" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="C47" s="51" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="D47" s="51" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="E47" s="51" t="s">
         <v>159</v>
       </c>
       <c r="F47" s="51" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="G47" s="51"/>
       <c r="H47" s="51">
@@ -10235,8 +10219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{874AFBB5-8FFB-B248-A4C3-9A81309B9614}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -10251,7 +10235,7 @@
         <v>374</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -10264,10 +10248,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -10275,7 +10259,7 @@
         <v>383</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>645</v>
+        <v>329</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -10283,7 +10267,7 @@
         <v>386</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>613</v>
+        <v>643</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -10307,7 +10291,7 @@
         <v>600</v>
       </c>
       <c r="B8" s="44" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -10315,7 +10299,7 @@
         <v>389</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -10339,7 +10323,7 @@
         <v>393</v>
       </c>
       <c r="B12" s="44" t="s">
-        <v>611</v>
+        <v>644</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -10347,7 +10331,7 @@
         <v>393</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>612</v>
+        <v>645</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -10355,7 +10339,7 @@
         <v>393</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>335</v>
+        <v>646</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -10363,7 +10347,7 @@
         <v>393</v>
       </c>
       <c r="B15" s="44" t="s">
-        <v>616</v>
+        <v>335</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -10371,7 +10355,7 @@
         <v>393</v>
       </c>
       <c r="B16" s="44" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -10379,7 +10363,7 @@
         <v>393</v>
       </c>
       <c r="B17" s="44" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -10387,7 +10371,7 @@
         <v>393</v>
       </c>
       <c r="B18" s="44" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -10395,7 +10379,7 @@
         <v>393</v>
       </c>
       <c r="B19" s="44" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -10403,11 +10387,16 @@
         <v>393</v>
       </c>
       <c r="B20" s="44" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="44"/>
+      <c r="A21" s="25" t="s">
+        <v>393</v>
+      </c>
+      <c r="B21" s="44" t="s">
+        <v>618</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B20">

</xml_diff>

<commit_message>
Merging different targets for COVID into a single graph.
</commit_message>
<xml_diff>
--- a/dashboard/data/watchdb.all_tables.xlsx
+++ b/dashboard/data/watchdb.all_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B72292-9838-BA47-8870-E3972E546152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665BFF87-CD21-B341-8C03-318630D51726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="5" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1558" uniqueCount="645">
   <si>
     <t>CharlestonWWTP-01</t>
   </si>
@@ -1880,24 +1880,6 @@
     <t>RNase P</t>
   </si>
   <si>
-    <t>S:E484K</t>
-  </si>
-  <si>
-    <t>S:E484K WT</t>
-  </si>
-  <si>
-    <t>S:HVdel69-70</t>
-  </si>
-  <si>
-    <t>S:HVdel69-70 WT</t>
-  </si>
-  <si>
-    <t>S:N501Y</t>
-  </si>
-  <si>
-    <t>S:N501Y WT</t>
-  </si>
-  <si>
     <t>TNFR</t>
   </si>
   <si>
@@ -1980,6 +1962,18 @@
   </si>
   <si>
     <t>SC2</t>
+  </si>
+  <si>
+    <t>Human Norovirus GII (HuNoV-GII)</t>
+  </si>
+  <si>
+    <t>ORF1_2</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Human Norovirus GI (HuNoV-GI)</t>
   </si>
 </sst>
 </file>
@@ -1989,7 +1983,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2131,7 +2125,14 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2181,7 +2182,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2281,7 +2282,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2300,6 +2300,8 @@
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2784,7 +2786,7 @@
         <v>60</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>340</v>
@@ -4073,21 +4075,21 @@
       <c r="G25" s="29" t="s">
         <v>368</v>
       </c>
-      <c r="H25" s="46">
+      <c r="H25" s="45">
         <v>-82.430654000000004</v>
       </c>
-      <c r="I25" s="46">
+      <c r="I25" s="45">
         <v>38.424089000000002</v>
       </c>
-      <c r="J25" s="46" t="s">
-        <v>627</v>
+      <c r="J25" s="45" t="s">
+        <v>621</v>
       </c>
       <c r="K25" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L25" s="33"/>
       <c r="M25" s="33" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="N25" s="33">
         <v>5</v>
@@ -4107,8 +4109,8 @@
       <c r="S25" s="32">
         <v>25703</v>
       </c>
-      <c r="T25" s="46" t="s">
-        <v>634</v>
+      <c r="T25" s="45" t="s">
+        <v>628</v>
       </c>
     </row>
     <row r="26" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -4147,7 +4149,7 @@
         <v>4000</v>
       </c>
       <c r="M26" s="33" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="N26" s="33">
         <v>24</v>
@@ -4167,8 +4169,8 @@
       <c r="S26" s="42">
         <v>25504</v>
       </c>
-      <c r="T26" s="47" t="s">
-        <v>635</v>
+      <c r="T26" s="46" t="s">
+        <v>629</v>
       </c>
     </row>
     <row r="27" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4191,21 +4193,21 @@
       <c r="G27" s="29" t="s">
         <v>368</v>
       </c>
-      <c r="H27" s="46">
+      <c r="H27" s="45">
         <v>-82.425917999999996</v>
       </c>
-      <c r="I27" s="46">
+      <c r="I27" s="45">
         <v>38.421745999999999</v>
       </c>
-      <c r="J27" s="46" t="s">
-        <v>628</v>
+      <c r="J27" s="45" t="s">
+        <v>622</v>
       </c>
       <c r="K27" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L27" s="33"/>
       <c r="M27" s="33" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="N27" s="33">
         <v>5</v>
@@ -4225,8 +4227,8 @@
       <c r="S27" s="32">
         <v>25703</v>
       </c>
-      <c r="T27" s="46" t="s">
-        <v>633</v>
+      <c r="T27" s="45" t="s">
+        <v>627</v>
       </c>
     </row>
     <row r="28" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4514,7 +4516,7 @@
         <v>25701</v>
       </c>
       <c r="T32" s="29" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
@@ -4574,7 +4576,7 @@
         <v>25537</v>
       </c>
       <c r="T33" s="29" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="34" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -4613,7 +4615,7 @@
         <v>7000</v>
       </c>
       <c r="M34" s="34" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="N34" s="34">
         <v>24</v>
@@ -4637,7 +4639,7 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="29" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="B35" s="29"/>
       <c r="C35" s="29" t="s">
@@ -4647,7 +4649,7 @@
         <v>103</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="F35" s="29" t="s">
         <v>340</v>
@@ -4707,7 +4709,7 @@
         <v>103</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="F36" s="29" t="s">
         <v>340</v>
@@ -4775,21 +4777,21 @@
       <c r="G37" s="29" t="s">
         <v>368</v>
       </c>
-      <c r="H37" s="46">
+      <c r="H37" s="45">
         <v>-82.425557700629597</v>
       </c>
-      <c r="I37" s="46">
+      <c r="I37" s="45">
         <v>38.422913110104098</v>
       </c>
-      <c r="J37" s="46" t="s">
-        <v>630</v>
+      <c r="J37" s="45" t="s">
+        <v>624</v>
       </c>
       <c r="K37" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L37" s="33"/>
       <c r="M37" s="34" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="N37" s="33">
         <v>5</v>
@@ -4831,21 +4833,21 @@
       <c r="G38" s="29" t="s">
         <v>368</v>
       </c>
-      <c r="H38" s="46">
+      <c r="H38" s="45">
         <v>-82.424907815220195</v>
       </c>
-      <c r="I38" s="46">
+      <c r="I38" s="45">
         <v>38.423076174075902</v>
       </c>
-      <c r="J38" s="46" t="s">
-        <v>631</v>
+      <c r="J38" s="45" t="s">
+        <v>625</v>
       </c>
       <c r="K38" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L38" s="33"/>
       <c r="M38" s="34" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="N38" s="33">
         <v>24</v>
@@ -4868,62 +4870,62 @@
       <c r="T38" s="29"/>
     </row>
     <row r="39" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="46" t="s">
-        <v>624</v>
-      </c>
-      <c r="B39" s="46"/>
-      <c r="C39" s="46" t="s">
+      <c r="A39" s="45" t="s">
+        <v>618</v>
+      </c>
+      <c r="B39" s="45"/>
+      <c r="C39" s="45" t="s">
         <v>352</v>
       </c>
-      <c r="D39" s="48" t="s">
+      <c r="D39" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="E39" s="46" t="s">
-        <v>625</v>
-      </c>
-      <c r="F39" s="46" t="s">
+      <c r="E39" s="45" t="s">
+        <v>619</v>
+      </c>
+      <c r="F39" s="45" t="s">
         <v>340</v>
       </c>
-      <c r="G39" s="46" t="s">
+      <c r="G39" s="45" t="s">
         <v>368</v>
       </c>
-      <c r="H39" s="46">
+      <c r="H39" s="45">
         <v>-81.867118796822695</v>
       </c>
-      <c r="I39" s="46">
+      <c r="I39" s="45">
         <v>38.537901317549398</v>
       </c>
-      <c r="J39" s="46" t="s">
-        <v>626</v>
-      </c>
-      <c r="K39" s="46" t="s">
+      <c r="J39" s="45" t="s">
+        <v>620</v>
+      </c>
+      <c r="K39" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="L39" s="49">
+      <c r="L39" s="48">
         <v>4900</v>
       </c>
-      <c r="M39" s="50" t="s">
+      <c r="M39" s="49" t="s">
         <v>338</v>
       </c>
-      <c r="N39" s="50">
+      <c r="N39" s="49">
         <v>48</v>
       </c>
-      <c r="O39" s="50">
+      <c r="O39" s="49">
         <v>333</v>
       </c>
-      <c r="P39" s="50">
+      <c r="P39" s="49">
         <v>1440</v>
       </c>
-      <c r="Q39" s="46" t="s">
+      <c r="Q39" s="45" t="s">
         <v>347</v>
       </c>
-      <c r="R39" s="46" t="s">
+      <c r="R39" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="S39" s="48">
+      <c r="S39" s="47">
         <v>25168</v>
       </c>
-      <c r="T39" s="46"/>
+      <c r="T39" s="45"/>
     </row>
     <row r="40" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
@@ -7351,9 +7353,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7706D3C3-8C4A-6E4A-999A-41BCCB2FAC67}">
   <dimension ref="A1:Z47"/>
   <sheetViews>
-    <sheetView zoomScale="133" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="133" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8532,7 +8534,7 @@
         <v>10</v>
       </c>
       <c r="I44" s="30">
-        <v>50000</v>
+        <v>33782</v>
       </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
@@ -8593,48 +8595,48 @@
       <c r="W46"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="51" t="s">
-        <v>638</v>
-      </c>
-      <c r="B47" s="52" t="s">
-        <v>639</v>
-      </c>
-      <c r="C47" s="51" t="s">
-        <v>625</v>
-      </c>
-      <c r="D47" s="51" t="s">
-        <v>640</v>
-      </c>
-      <c r="E47" s="51" t="s">
+      <c r="A47" s="50" t="s">
+        <v>632</v>
+      </c>
+      <c r="B47" s="51" t="s">
+        <v>633</v>
+      </c>
+      <c r="C47" s="50" t="s">
+        <v>619</v>
+      </c>
+      <c r="D47" s="50" t="s">
+        <v>634</v>
+      </c>
+      <c r="E47" s="50" t="s">
         <v>159</v>
       </c>
-      <c r="F47" s="51" t="s">
-        <v>641</v>
-      </c>
-      <c r="G47" s="51"/>
-      <c r="H47" s="51">
+      <c r="F47" s="50" t="s">
+        <v>635</v>
+      </c>
+      <c r="G47" s="50"/>
+      <c r="H47" s="50">
         <v>0.3</v>
       </c>
-      <c r="I47" s="53">
+      <c r="I47" s="52">
         <v>3500</v>
       </c>
-      <c r="J47" s="52"/>
-      <c r="K47" s="52"/>
-      <c r="L47" s="52"/>
-      <c r="M47" s="52"/>
-      <c r="N47" s="52"/>
-      <c r="O47" s="52"/>
-      <c r="P47" s="52"/>
-      <c r="Q47" s="52"/>
-      <c r="R47" s="52"/>
-      <c r="S47" s="52"/>
-      <c r="T47" s="52"/>
-      <c r="U47" s="52"/>
-      <c r="V47" s="52"/>
-      <c r="W47" s="52"/>
-      <c r="X47" s="52"/>
-      <c r="Y47" s="52"/>
-      <c r="Z47" s="52"/>
+      <c r="J47" s="51"/>
+      <c r="K47" s="51"/>
+      <c r="L47" s="51"/>
+      <c r="M47" s="51"/>
+      <c r="N47" s="51"/>
+      <c r="O47" s="51"/>
+      <c r="P47" s="51"/>
+      <c r="Q47" s="51"/>
+      <c r="R47" s="51"/>
+      <c r="S47" s="51"/>
+      <c r="T47" s="51"/>
+      <c r="U47" s="51"/>
+      <c r="V47" s="51"/>
+      <c r="W47" s="51"/>
+      <c r="X47" s="51"/>
+      <c r="Y47" s="51"/>
+      <c r="Z47" s="51"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I46">
@@ -8649,7 +8651,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8728,7 +8730,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="18">
-        <v>41411</v>
+        <v>41447</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -10219,13 +10221,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{874AFBB5-8FFB-B248-A4C3-9A81309B9614}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" style="25" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="25"/>
   </cols>
@@ -10235,7 +10237,7 @@
         <v>374</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -10248,14 +10250,14 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="B3" s="44" t="s">
         <v>612</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="44" t="s">
         <v>383</v>
       </c>
       <c r="B4" s="44" t="s">
@@ -10263,11 +10265,11 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="44" t="s">
         <v>386</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -10279,7 +10281,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="44" t="s">
         <v>599</v>
       </c>
       <c r="B7" s="44" t="s">
@@ -10287,27 +10289,27 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="44" t="s">
         <v>600</v>
       </c>
       <c r="B8" s="44" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>611</v>
+        <v>638</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>323</v>
+        <v>639</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -10315,88 +10317,68 @@
         <v>393</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>321</v>
+        <v>640</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
-        <v>393</v>
-      </c>
-      <c r="B12" s="44" t="s">
-        <v>644</v>
+        <v>593</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
-        <v>393</v>
-      </c>
-      <c r="B13" s="44" t="s">
-        <v>645</v>
+        <v>641</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>642</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
-        <v>393</v>
-      </c>
-      <c r="B14" s="44" t="s">
-        <v>646</v>
+      <c r="A14" s="53" t="s">
+        <v>592</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>643</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
-        <v>393</v>
-      </c>
-      <c r="B15" s="44" t="s">
-        <v>335</v>
+      <c r="A15" s="54" t="s">
+        <v>588</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>643</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
-        <v>393</v>
-      </c>
-      <c r="B16" s="44" t="s">
-        <v>613</v>
+      <c r="A16" s="54" t="s">
+        <v>589</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>643</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
-        <v>393</v>
-      </c>
-      <c r="B17" s="44" t="s">
-        <v>614</v>
+      <c r="A17" s="53" t="s">
+        <v>644</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>611</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
-        <v>393</v>
-      </c>
-      <c r="B18" s="44" t="s">
-        <v>615</v>
-      </c>
+      <c r="B18" s="44"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
-        <v>393</v>
-      </c>
-      <c r="B19" s="44" t="s">
-        <v>616</v>
-      </c>
+      <c r="B19" s="44"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
-        <v>393</v>
-      </c>
-      <c r="B20" s="44" t="s">
-        <v>617</v>
-      </c>
+      <c r="B20" s="44"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
-        <v>393</v>
-      </c>
-      <c r="B21" s="44" t="s">
-        <v>618</v>
-      </c>
+      <c r="B21" s="44"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B20">

</xml_diff>

<commit_message>
Data update. Added dashboard_ignore field to NWSS update to accomodate MU binned samples. Started adding smarter lab_method encoding but not implemented yet.
</commit_message>
<xml_diff>
--- a/dashboard/data/watchdb.all_tables.xlsx
+++ b/dashboard/data/watchdb.all_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/dashboard/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665BFF87-CD21-B341-8C03-318630D51726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A186F5C-AB50-C84B-956D-BAA8892ABE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="19780" yWindow="500" windowWidth="30240" windowHeight="18880" activeTab="6" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="target" sheetId="4" r:id="rId4"/>
     <sheet name="lab" sheetId="5" r:id="rId5"/>
     <sheet name="loci" sheetId="6" r:id="rId6"/>
+    <sheet name="methods" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1558" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="651">
   <si>
     <t>CharlestonWWTP-01</t>
   </si>
@@ -1974,6 +1975,24 @@
   </si>
   <si>
     <t>Human Norovirus GI (HuNoV-GI)</t>
+  </si>
+  <si>
+    <t>major_lab_method</t>
+  </si>
+  <si>
+    <t>major_lab_method_desc</t>
+  </si>
+  <si>
+    <t>Nanotrap concentration of raw influent and quantification by ddPCR</t>
+  </si>
+  <si>
+    <t>Nanotrap concentration of raw influent and quantification by ddPCR; the only modification from major_lab_method 1 is that post-RNA extraction, four equal volumes of RNA extract are combined for ddPCR analysis, rather than being combined pre-concentration.</t>
+  </si>
+  <si>
+    <t>Nanotrap concentration of raw influent and quantification by ddPCR; the only modification from major_lab_method 1 is that post-RNA extraction, two equal volumes of RNA extract are combined for ddPCR analysis, rather than being combined pre-concentration.</t>
+  </si>
+  <si>
+    <t>Nanotrap concentration of raw influent and quantification by ddPCR; the only modification from major_lab_method 1 is that post-RNA extraction, three equal volumes of RNA extract are combined for ddPCR analysis, rather than being combined pre-concentration.</t>
   </si>
 </sst>
 </file>
@@ -2182,7 +2201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2302,6 +2321,12 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -7353,7 +7378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7706D3C3-8C4A-6E4A-999A-41BCCB2FAC67}">
   <dimension ref="A1:Z47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="133" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="133" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I44" sqref="I44"/>
     </sheetView>
@@ -10386,4 +10411,75 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5881ED24-91ED-D44B-B541-ADE5F93B4B89}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="106.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="55" t="s">
+        <v>645</v>
+      </c>
+      <c r="B1" s="55" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="56">
+        <v>1</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="56">
+        <v>2</v>
+      </c>
+      <c r="B3" s="56" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="56">
+        <v>3</v>
+      </c>
+      <c r="B4" s="56"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="56">
+        <v>4</v>
+      </c>
+      <c r="B5" s="56"/>
+    </row>
+    <row r="6" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="56">
+        <v>5</v>
+      </c>
+      <c r="B6" s="56" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="56">
+        <v>6</v>
+      </c>
+      <c r="B7" s="56" t="s">
+        <v>650</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Data update plus clean out of backed-up data.
</commit_message>
<xml_diff>
--- a/dashboard/data/watchdb.all_tables.xlsx
+++ b/dashboard/data/watchdb.all_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA468563-08FF-834B-9CC4-BAF89E358689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEAB7F64-85C7-FA47-BF83-2DC605A74F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="51960" yWindow="4820" windowWidth="30240" windowHeight="18880" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1554" uniqueCount="625">
   <si>
     <t>CharlestonWWTP-01</t>
   </si>
@@ -1344,105 +1344,6 @@
     <t>V</t>
   </si>
   <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Z</t>
-  </si>
-  <si>
-    <t>AA</t>
-  </si>
-  <si>
-    <t>BB</t>
-  </si>
-  <si>
-    <t>CC</t>
-  </si>
-  <si>
-    <t>DD</t>
-  </si>
-  <si>
-    <t>EE</t>
-  </si>
-  <si>
-    <t>FF</t>
-  </si>
-  <si>
-    <t>GG</t>
-  </si>
-  <si>
-    <t>HH</t>
-  </si>
-  <si>
-    <t>II</t>
-  </si>
-  <si>
-    <t>JJ</t>
-  </si>
-  <si>
-    <t>KK</t>
-  </si>
-  <si>
-    <t>LL</t>
-  </si>
-  <si>
-    <t>MM</t>
-  </si>
-  <si>
-    <t>NN</t>
-  </si>
-  <si>
-    <t>OO</t>
-  </si>
-  <si>
-    <t>PP</t>
-  </si>
-  <si>
-    <t>QQ</t>
-  </si>
-  <si>
-    <t>RR</t>
-  </si>
-  <si>
-    <t>SS</t>
-  </si>
-  <si>
-    <t>TT</t>
-  </si>
-  <si>
-    <t>UU</t>
-  </si>
-  <si>
-    <t>VV</t>
-  </si>
-  <si>
-    <t>WW</t>
-  </si>
-  <si>
-    <t>XX</t>
-  </si>
-  <si>
-    <t>YY</t>
-  </si>
-  <si>
-    <t>ZZ</t>
-  </si>
-  <si>
-    <t>AAA</t>
-  </si>
-  <si>
-    <t>BBB</t>
-  </si>
-  <si>
-    <t>CCC</t>
-  </si>
-  <si>
     <t>StadiumSW-01</t>
   </si>
   <si>
@@ -1996,6 +1897,24 @@
   </si>
   <si>
     <t>huNovGI</t>
+  </si>
+  <si>
+    <t>MoorefieldWWTP-01</t>
+  </si>
+  <si>
+    <t>Moorefield</t>
+  </si>
+  <si>
+    <t>MoorefieldWWTP</t>
+  </si>
+  <si>
+    <t>Moorefield WWTP</t>
+  </si>
+  <si>
+    <t>V01</t>
+  </si>
+  <si>
+    <t>54029-001-01-00-00</t>
   </si>
 </sst>
 </file>
@@ -2005,7 +1924,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2158,6 +2077,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -2204,7 +2128,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2329,6 +2253,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2650,13 +2586,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0856F7A-D0C0-3942-9027-9FB2F3C2C3E0}">
-  <dimension ref="A1:T81"/>
+  <dimension ref="A1:T82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D64" sqref="D61:D64"/>
+      <selection pane="bottomRight" activeCell="Q83" sqref="Q83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2683,7 +2619,7 @@
         <v>191</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>541</v>
+        <v>508</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>349</v>
@@ -2946,7 +2882,7 @@
         <v>7000</v>
       </c>
       <c r="M5" s="34" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="N5" s="34">
         <v>24</v>
@@ -2970,7 +2906,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="45" t="s">
-        <v>618</v>
+        <v>585</v>
       </c>
       <c r="B6" s="45"/>
       <c r="C6" s="45" t="s">
@@ -2980,7 +2916,7 @@
         <v>103</v>
       </c>
       <c r="E6" s="45" t="s">
-        <v>619</v>
+        <v>586</v>
       </c>
       <c r="F6" s="45" t="s">
         <v>340</v>
@@ -2995,7 +2931,7 @@
         <v>38.537901317549398</v>
       </c>
       <c r="J6" s="45" t="s">
-        <v>620</v>
+        <v>587</v>
       </c>
       <c r="K6" s="45" t="s">
         <v>159</v>
@@ -3028,7 +2964,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
-        <v>623</v>
+        <v>590</v>
       </c>
       <c r="B7" s="29"/>
       <c r="C7" s="29" t="s">
@@ -3038,7 +2974,7 @@
         <v>103</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>616</v>
+        <v>583</v>
       </c>
       <c r="F7" s="29" t="s">
         <v>340</v>
@@ -3098,7 +3034,7 @@
         <v>103</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>615</v>
+        <v>582</v>
       </c>
       <c r="F8" s="29" t="s">
         <v>340</v>
@@ -3151,7 +3087,7 @@
         <v>62</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>542</v>
+        <v>509</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>351</v>
@@ -3212,7 +3148,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>567</v>
+        <v>534</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>351</v>
@@ -3268,7 +3204,7 @@
         <v>101</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>568</v>
+        <v>535</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>351</v>
@@ -3328,7 +3264,7 @@
         <v>93</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>549</v>
+        <v>516</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>351</v>
@@ -3381,10 +3317,10 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>475</v>
+        <v>442</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>351</v>
@@ -3393,7 +3329,7 @@
         <v>103</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>476</v>
+        <v>443</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>341</v>
@@ -3442,7 +3378,7 @@
         <v>113</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>550</v>
+        <v>517</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>351</v>
@@ -3502,7 +3438,7 @@
         <v>109</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>583</v>
+        <v>550</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>351</v>
@@ -3562,7 +3498,7 @@
         <v>99</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>553</v>
+        <v>520</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>351</v>
@@ -3618,7 +3554,7 @@
         <v>108</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>554</v>
+        <v>521</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>351</v>
@@ -3678,7 +3614,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>555</v>
+        <v>522</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>351</v>
@@ -3738,7 +3674,7 @@
         <v>152</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>556</v>
+        <v>523</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>351</v>
@@ -3798,7 +3734,7 @@
         <v>104</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>551</v>
+        <v>518</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>351</v>
@@ -3858,7 +3794,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>557</v>
+        <v>524</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>351</v>
@@ -3913,7 +3849,7 @@
         <v>49</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>558</v>
+        <v>525</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>351</v>
@@ -3969,7 +3905,7 @@
         <v>188</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>559</v>
+        <v>526</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>351</v>
@@ -4028,7 +3964,7 @@
         <v>16</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>561</v>
+        <v>528</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>351</v>
@@ -4088,7 +4024,7 @@
         <v>106</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>562</v>
+        <v>529</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>351</v>
@@ -4147,7 +4083,7 @@
         <v>10</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>544</v>
+        <v>511</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>351</v>
@@ -4203,7 +4139,7 @@
         <v>52</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>558</v>
+        <v>525</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>351</v>
@@ -4263,7 +4199,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>566</v>
+        <v>533</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>351</v>
@@ -4316,10 +4252,10 @@
     </row>
     <row r="29" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
-        <v>477</v>
+        <v>444</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>543</v>
+        <v>510</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>351</v>
@@ -4328,7 +4264,7 @@
         <v>103</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>478</v>
+        <v>445</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>340</v>
@@ -4343,7 +4279,7 @@
         <v>37.946770700000002</v>
       </c>
       <c r="J29" s="12" t="s">
-        <v>584</v>
+        <v>551</v>
       </c>
       <c r="K29" s="12" t="s">
         <v>197</v>
@@ -4401,14 +4337,14 @@
         <v>38.424089000000002</v>
       </c>
       <c r="J30" s="45" t="s">
-        <v>621</v>
+        <v>588</v>
       </c>
       <c r="K30" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L30" s="33"/>
       <c r="M30" s="33" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="N30" s="33">
         <v>5</v>
@@ -4429,7 +4365,7 @@
         <v>25703</v>
       </c>
       <c r="T30" s="45" t="s">
-        <v>628</v>
+        <v>595</v>
       </c>
     </row>
     <row r="31" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -4468,7 +4404,7 @@
         <v>4000</v>
       </c>
       <c r="M31" s="33" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="N31" s="33">
         <v>24</v>
@@ -4489,7 +4425,7 @@
         <v>25504</v>
       </c>
       <c r="T31" s="46" t="s">
-        <v>629</v>
+        <v>596</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
@@ -4519,14 +4455,14 @@
         <v>38.421745999999999</v>
       </c>
       <c r="J32" s="45" t="s">
-        <v>622</v>
+        <v>589</v>
       </c>
       <c r="K32" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L32" s="33"/>
       <c r="M32" s="33" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="N32" s="33">
         <v>5</v>
@@ -4547,7 +4483,7 @@
         <v>25703</v>
       </c>
       <c r="T32" s="45" t="s">
-        <v>627</v>
+        <v>594</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
@@ -4665,7 +4601,7 @@
         <v>25701</v>
       </c>
       <c r="T34" s="29" t="s">
-        <v>630</v>
+        <v>597</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
@@ -4725,7 +4661,7 @@
         <v>25537</v>
       </c>
       <c r="T35" s="29" t="s">
-        <v>631</v>
+        <v>598</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
@@ -4755,14 +4691,14 @@
         <v>38.422913110104098</v>
       </c>
       <c r="J36" s="45" t="s">
-        <v>624</v>
+        <v>591</v>
       </c>
       <c r="K36" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L36" s="33"/>
       <c r="M36" s="34" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="N36" s="33">
         <v>5</v>
@@ -4811,14 +4747,14 @@
         <v>38.423076174075902</v>
       </c>
       <c r="J37" s="45" t="s">
-        <v>625</v>
+        <v>592</v>
       </c>
       <c r="K37" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L37" s="33"/>
       <c r="M37" s="34" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="N37" s="33">
         <v>24</v>
@@ -4845,7 +4781,7 @@
         <v>18</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>547</v>
+        <v>514</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>351</v>
@@ -4905,7 +4841,7 @@
         <v>35</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>546</v>
+        <v>513</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>351</v>
@@ -4961,7 +4897,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>548</v>
+        <v>515</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>351</v>
@@ -4970,7 +4906,7 @@
         <v>60</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>617</v>
+        <v>584</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>340</v>
@@ -5017,7 +4953,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>546</v>
+        <v>513</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>351</v>
@@ -5073,7 +5009,7 @@
         <v>21</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>351</v>
@@ -5135,7 +5071,7 @@
         <v>25</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>351</v>
@@ -5197,7 +5133,7 @@
         <v>26</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>351</v>
@@ -5259,7 +5195,7 @@
         <v>22</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>351</v>
@@ -5319,7 +5255,7 @@
         <v>27</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>351</v>
@@ -5379,7 +5315,7 @@
         <v>28</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>351</v>
@@ -5439,7 +5375,7 @@
         <v>111</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>552</v>
+        <v>519</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>351</v>
@@ -5550,7 +5486,7 @@
         <v>192</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>351</v>
@@ -5612,7 +5548,7 @@
         <v>29</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>351</v>
@@ -5672,7 +5608,7 @@
         <v>30</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>351</v>
@@ -5732,7 +5668,7 @@
         <v>38</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>546</v>
+        <v>513</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>351</v>
@@ -5787,7 +5723,7 @@
         <v>39</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>546</v>
+        <v>513</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>351</v>
@@ -5842,7 +5778,7 @@
         <v>31</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>351</v>
@@ -5902,7 +5838,7 @@
         <v>36</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>351</v>
@@ -5957,7 +5893,7 @@
         <v>339</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>351</v>
@@ -6017,7 +5953,7 @@
         <v>23</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>351</v>
@@ -6133,7 +6069,7 @@
         <v>184</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>351</v>
@@ -6192,10 +6128,10 @@
     </row>
     <row r="61" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>471</v>
+        <v>438</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>351</v>
@@ -6204,7 +6140,7 @@
         <v>103</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>472</v>
+        <v>439</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>341</v>
@@ -6246,10 +6182,10 @@
     </row>
     <row r="62" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>351</v>
@@ -6258,7 +6194,7 @@
         <v>103</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>470</v>
+        <v>437</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>341</v>
@@ -6300,10 +6236,10 @@
     </row>
     <row r="63" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>473</v>
+        <v>440</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>351</v>
@@ -6312,7 +6248,7 @@
         <v>103</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>474</v>
+        <v>441</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>341</v>
@@ -6354,10 +6290,10 @@
     </row>
     <row r="64" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>467</v>
+        <v>434</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>351</v>
@@ -6366,7 +6302,7 @@
         <v>103</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>468</v>
+        <v>435</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>341</v>
@@ -6411,7 +6347,7 @@
         <v>51</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>563</v>
+        <v>530</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>351</v>
@@ -6471,7 +6407,7 @@
         <v>58</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>546</v>
+        <v>513</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>351</v>
@@ -6527,7 +6463,7 @@
         <v>24</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>351</v>
@@ -6589,7 +6525,7 @@
         <v>37</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>546</v>
+        <v>513</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>351</v>
@@ -6645,7 +6581,7 @@
         <v>32</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>351</v>
@@ -6705,7 +6641,7 @@
         <v>8</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>565</v>
+        <v>532</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>351</v>
@@ -6765,7 +6701,7 @@
         <v>33</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>351</v>
@@ -7103,7 +7039,7 @@
         <v>59</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>560</v>
+        <v>527</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>351</v>
@@ -7211,7 +7147,7 @@
         <v>14</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>564</v>
+        <v>531</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>351</v>
@@ -7366,6 +7302,59 @@
         <v>26591</v>
       </c>
       <c r="T81" s="2"/>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="B82" t="s">
+        <v>623</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="H82" s="2">
+        <v>-78.955160000000006</v>
+      </c>
+      <c r="I82" s="2">
+        <v>39.115929999999999</v>
+      </c>
+      <c r="J82" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="K82" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="L82" s="38">
+        <v>3510</v>
+      </c>
+      <c r="M82" s="38" t="s">
+        <v>338</v>
+      </c>
+      <c r="N82" s="38">
+        <v>24</v>
+      </c>
+      <c r="Q82" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="R82" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S82" s="1">
+        <v>26836</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T81">
@@ -7379,16 +7368,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7706D3C3-8C4A-6E4A-999A-41BCCB2FAC67}">
-  <dimension ref="A1:Z47"/>
+  <dimension ref="A1:Z48"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="133" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I44" sqref="I44"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.83203125" customWidth="1"/>
     <col min="3" max="3" width="32.33203125" customWidth="1"/>
     <col min="4" max="5" width="23.83203125" customWidth="1"/>
@@ -7403,7 +7392,7 @@
         <v>230</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>504</v>
+        <v>471</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>229</v>
@@ -7415,7 +7404,7 @@
         <v>238</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>480</v>
+        <v>447</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>240</v>
@@ -7432,7 +7421,7 @@
         <v>275</v>
       </c>
       <c r="B2" t="s">
-        <v>505</v>
+        <v>472</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>64</v>
@@ -7444,7 +7433,7 @@
         <v>63</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>481</v>
+        <v>448</v>
       </c>
       <c r="G2" s="31">
         <v>54003906001</v>
@@ -7462,7 +7451,7 @@
         <v>244</v>
       </c>
       <c r="B3" t="s">
-        <v>506</v>
+        <v>473</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>277</v>
@@ -7474,7 +7463,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>482</v>
+        <v>449</v>
       </c>
       <c r="G3" s="17">
         <v>54002701001</v>
@@ -7499,7 +7488,7 @@
         <v>157</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>573</v>
+        <v>540</v>
       </c>
       <c r="G4" s="31">
         <v>54000601001</v>
@@ -7526,7 +7515,7 @@
         <v>123</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>574</v>
+        <v>541</v>
       </c>
       <c r="G5" s="31">
         <v>54000101001</v>
@@ -7553,7 +7542,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>575</v>
+        <v>542</v>
       </c>
       <c r="G6" s="31">
         <v>54003031001</v>
@@ -7580,7 +7569,7 @@
         <v>88</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>576</v>
+        <v>543</v>
       </c>
       <c r="G7" s="31">
         <v>54001702001</v>
@@ -7605,7 +7594,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>577</v>
+        <v>544</v>
       </c>
       <c r="G8" s="31">
         <v>54002510001</v>
@@ -7622,7 +7611,7 @@
         <v>357</v>
       </c>
       <c r="B9" t="s">
-        <v>508</v>
+        <v>475</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>362</v>
@@ -7632,7 +7621,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>536</v>
+        <v>503</v>
       </c>
       <c r="G9" s="31">
         <v>54002003001</v>
@@ -7649,7 +7638,7 @@
         <v>249</v>
       </c>
       <c r="B10" t="s">
-        <v>507</v>
+        <v>474</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>282</v>
@@ -7659,7 +7648,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>483</v>
+        <v>450</v>
       </c>
       <c r="G10" s="31">
         <v>54002003001</v>
@@ -7676,7 +7665,7 @@
         <v>250</v>
       </c>
       <c r="B11" t="s">
-        <v>509</v>
+        <v>476</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>283</v>
@@ -7686,7 +7675,7 @@
         <v>7</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>484</v>
+        <v>451</v>
       </c>
       <c r="G11" s="31">
         <v>54001901001</v>
@@ -7703,7 +7692,7 @@
         <v>251</v>
       </c>
       <c r="B12" t="s">
-        <v>510</v>
+        <v>477</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>306</v>
@@ -7715,7 +7704,7 @@
         <v>11</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>485</v>
+        <v>452</v>
       </c>
       <c r="G12" s="31">
         <v>54003045001</v>
@@ -7732,7 +7721,7 @@
         <v>252</v>
       </c>
       <c r="B13" t="s">
-        <v>511</v>
+        <v>478</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>284</v>
@@ -7742,7 +7731,7 @@
         <v>88</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>486</v>
+        <v>453</v>
       </c>
       <c r="G13" s="31">
         <v>54001703001</v>
@@ -7759,7 +7748,7 @@
         <v>358</v>
       </c>
       <c r="B14" t="s">
-        <v>512</v>
+        <v>479</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>363</v>
@@ -7769,7 +7758,7 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>537</v>
+        <v>504</v>
       </c>
       <c r="G14" s="31">
         <v>54002007001</v>
@@ -7786,7 +7775,7 @@
         <v>253</v>
       </c>
       <c r="B15" t="s">
-        <v>513</v>
+        <v>480</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>285</v>
@@ -7796,7 +7785,7 @@
         <v>121</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>487</v>
+        <v>454</v>
       </c>
       <c r="G15" s="31">
         <v>54004202001</v>
@@ -7821,7 +7810,7 @@
         <v>89</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>578</v>
+        <v>545</v>
       </c>
       <c r="G16" s="31">
         <v>54002405001</v>
@@ -7838,7 +7827,7 @@
         <v>255</v>
       </c>
       <c r="B17" t="s">
-        <v>514</v>
+        <v>481</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>287</v>
@@ -7848,7 +7837,7 @@
         <v>89</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>579</v>
+        <v>546</v>
       </c>
       <c r="G17" s="31">
         <v>54002408001</v>
@@ -7865,7 +7854,7 @@
         <v>256</v>
       </c>
       <c r="B18" t="s">
-        <v>515</v>
+        <v>482</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>288</v>
@@ -7875,7 +7864,7 @@
         <v>122</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>488</v>
+        <v>455</v>
       </c>
       <c r="G18" s="17">
         <v>54000504001</v>
@@ -7892,7 +7881,7 @@
         <v>257</v>
       </c>
       <c r="B19" t="s">
-        <v>516</v>
+        <v>483</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>289</v>
@@ -7902,7 +7891,7 @@
         <v>100</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>489</v>
+        <v>456</v>
       </c>
       <c r="G19" s="31">
         <v>54004602001</v>
@@ -7938,240 +7927,246 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="s">
-        <v>353</v>
-      </c>
-      <c r="B21" t="s">
-        <v>517</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>360</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>361</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="F21" t="s">
-        <v>538</v>
-      </c>
-      <c r="G21" s="31">
-        <v>54000603001</v>
-      </c>
-      <c r="H21" s="17">
-        <v>17</v>
-      </c>
-      <c r="I21" s="17">
-        <v>56000</v>
+      <c r="A21" s="50" t="s">
+        <v>599</v>
+      </c>
+      <c r="B21" s="51" t="s">
+        <v>600</v>
+      </c>
+      <c r="C21" s="50" t="s">
+        <v>586</v>
+      </c>
+      <c r="D21" s="50" t="s">
+        <v>601</v>
+      </c>
+      <c r="E21" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="F21" s="50" t="s">
+        <v>602</v>
+      </c>
+      <c r="G21" s="50"/>
+      <c r="H21" s="50">
+        <v>0.3</v>
+      </c>
+      <c r="I21" s="52">
+        <v>3500</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>258</v>
+        <v>353</v>
       </c>
       <c r="B22" t="s">
-        <v>518</v>
+        <v>484</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="D22" s="17"/>
+        <v>360</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>361</v>
+      </c>
       <c r="E22" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>490</v>
+        <v>182</v>
+      </c>
+      <c r="F22" t="s">
+        <v>505</v>
       </c>
       <c r="G22" s="31">
-        <v>54004215001</v>
+        <v>54000603001</v>
       </c>
       <c r="H22" s="17">
-        <v>0.41</v>
-      </c>
-      <c r="I22" s="30">
-        <v>2101</v>
+        <v>17</v>
+      </c>
+      <c r="I22" s="17">
+        <v>56000</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>243</v>
+        <v>258</v>
       </c>
       <c r="B23" t="s">
-        <v>519</v>
+        <v>485</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="17" t="s">
-        <v>13</v>
+        <v>121</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>580</v>
+        <v>457</v>
       </c>
       <c r="G23" s="31">
-        <v>54002803001</v>
+        <v>54004215001</v>
       </c>
       <c r="H23" s="17">
-        <v>2.4</v>
+        <v>0.41</v>
       </c>
       <c r="I23" s="30">
-        <v>8168</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="B24" t="s">
-        <v>520</v>
+        <v>486</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="17" t="s">
-        <v>153</v>
+        <v>13</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>491</v>
+        <v>547</v>
       </c>
       <c r="G24" s="31">
-        <v>54000316001</v>
+        <v>54002803001</v>
       </c>
       <c r="H24" s="17">
-        <v>0.5</v>
+        <v>2.4</v>
       </c>
       <c r="I24" s="30">
-        <v>4555</v>
+        <v>8168</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B25" t="s">
-        <v>521</v>
+        <v>487</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D25" s="17"/>
       <c r="E25" s="17" t="s">
-        <v>89</v>
+        <v>153</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>492</v>
+        <v>458</v>
       </c>
       <c r="G25" s="31">
-        <v>54002415001</v>
+        <v>54000316001</v>
       </c>
       <c r="H25" s="17">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="I25" s="30">
-        <v>1091</v>
+        <v>4555</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B26" t="s">
-        <v>522</v>
+        <v>488</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="17" t="s">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>493</v>
+        <v>459</v>
       </c>
       <c r="G26" s="31">
-        <v>54002509001</v>
+        <v>54002415001</v>
       </c>
       <c r="H26" s="17">
-        <v>2.34</v>
+        <v>0.25</v>
       </c>
       <c r="I26" s="30">
-        <v>12000</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B27" t="s">
-        <v>523</v>
+        <v>489</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D27" s="17"/>
       <c r="E27" s="17" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>494</v>
+        <v>460</v>
       </c>
       <c r="G27" s="31">
-        <v>54005405001</v>
+        <v>54002509001</v>
       </c>
       <c r="H27" s="17">
-        <v>15.5</v>
+        <v>2.34</v>
       </c>
       <c r="I27" s="30">
-        <v>48050</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>355</v>
+        <v>262</v>
       </c>
       <c r="B28" t="s">
-        <v>524</v>
+        <v>490</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>365</v>
+        <v>296</v>
       </c>
       <c r="D28" s="17"/>
       <c r="E28" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="F28" t="s">
-        <v>539</v>
-      </c>
-      <c r="G28" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="G28" s="31">
+        <v>54005405001</v>
+      </c>
       <c r="H28" s="17">
-        <v>2.16</v>
-      </c>
-      <c r="I28" s="17">
-        <v>7000</v>
+        <v>15.5</v>
+      </c>
+      <c r="I28" s="30">
+        <v>48050</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>354</v>
-      </c>
-      <c r="B29" s="17"/>
+        <v>355</v>
+      </c>
+      <c r="B29" t="s">
+        <v>491</v>
+      </c>
       <c r="C29" s="17" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D29" s="17"/>
       <c r="E29" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
+      <c r="F29" t="s">
+        <v>506</v>
+      </c>
+      <c r="G29" s="4"/>
       <c r="H29" s="17">
-        <v>0.125</v>
+        <v>2.16</v>
       </c>
       <c r="I29" s="17">
-        <v>1000</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -8182,437 +8177,435 @@
       <c r="C30" s="17" t="s">
         <v>366</v>
       </c>
-      <c r="D30" s="4"/>
+      <c r="D30" s="17"/>
       <c r="E30" s="17" t="s">
         <v>157</v>
       </c>
       <c r="F30" s="17"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4">
+      <c r="G30" s="17"/>
+      <c r="H30" s="17">
         <v>0.125</v>
       </c>
-      <c r="I30" s="4">
+      <c r="I30" s="17">
         <v>1000</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>263</v>
+        <v>354</v>
       </c>
       <c r="B31" s="17"/>
       <c r="C31" s="17" t="s">
-        <v>297</v>
-      </c>
-      <c r="D31" s="17"/>
+        <v>366</v>
+      </c>
+      <c r="D31" s="4"/>
       <c r="E31" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F31" s="17" t="s">
-        <v>572</v>
-      </c>
-      <c r="G31" s="17">
-        <v>54001205001</v>
-      </c>
-      <c r="H31" s="17">
-        <v>1.35</v>
-      </c>
-      <c r="I31" s="30">
-        <v>2700</v>
+        <v>157</v>
+      </c>
+      <c r="F31" s="17"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4">
+        <v>0.125</v>
+      </c>
+      <c r="I31" s="4">
+        <v>1000</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
-        <v>264</v>
-      </c>
-      <c r="B32" t="s">
-        <v>525</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="B32" s="17"/>
       <c r="C32" s="17" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="D32" s="17"/>
       <c r="E32" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>495</v>
+        <v>55</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>539</v>
       </c>
       <c r="G32" s="17">
-        <v>54002606001</v>
+        <v>54001205001</v>
       </c>
       <c r="H32" s="17">
-        <v>0.7</v>
+        <v>1.35</v>
       </c>
       <c r="I32" s="30">
-        <v>5515</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B33" t="s">
-        <v>526</v>
+        <v>492</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="D33" s="17"/>
       <c r="E33" s="17" t="s">
-        <v>17</v>
+        <v>190</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>496</v>
+        <v>462</v>
       </c>
       <c r="G33" s="17">
-        <v>54002716001</v>
+        <v>54002606001</v>
       </c>
       <c r="H33" s="17">
-        <v>4.9000000000000004</v>
+        <v>0.7</v>
       </c>
       <c r="I33" s="30">
-        <v>36000</v>
+        <v>5515</v>
       </c>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B34" t="s">
-        <v>527</v>
+        <v>493</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D34" s="17"/>
       <c r="E34" s="17" t="s">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>497</v>
-      </c>
-      <c r="G34" s="31">
-        <v>54001710001</v>
+        <v>463</v>
+      </c>
+      <c r="G34" s="17">
+        <v>54002716001</v>
       </c>
       <c r="H34" s="17">
-        <v>0.4</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I34" s="30">
-        <v>1853</v>
+        <v>36000</v>
       </c>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
-        <v>370</v>
+        <v>266</v>
       </c>
       <c r="B35" t="s">
-        <v>528</v>
+        <v>494</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>372</v>
+        <v>299</v>
       </c>
       <c r="D35" s="17"/>
       <c r="E35" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="F35" t="s">
-        <v>540</v>
-      </c>
-      <c r="G35" s="4"/>
+        <v>88</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="G35" s="31">
+        <v>54001710001</v>
+      </c>
       <c r="H35" s="17">
-        <v>1.8</v>
-      </c>
-      <c r="I35" s="17">
-        <v>7200</v>
+        <v>0.4</v>
+      </c>
+      <c r="I35" s="30">
+        <v>1853</v>
       </c>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B36" t="s">
-        <v>529</v>
+        <v>495</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D36" s="17"/>
       <c r="E36" s="17" t="s">
         <v>157</v>
       </c>
       <c r="F36" t="s">
-        <v>540</v>
-      </c>
-      <c r="G36" s="17"/>
+        <v>507</v>
+      </c>
+      <c r="G36" s="4"/>
       <c r="H36" s="17">
-        <v>0.7</v>
+        <v>1.8</v>
       </c>
       <c r="I36" s="17">
-        <v>4050</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
-        <v>267</v>
-      </c>
-      <c r="B37" s="17"/>
+        <v>371</v>
+      </c>
+      <c r="B37" t="s">
+        <v>496</v>
+      </c>
       <c r="C37" s="17" t="s">
-        <v>300</v>
+        <v>373</v>
       </c>
       <c r="D37" s="17"/>
       <c r="E37" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>581</v>
-      </c>
-      <c r="G37" s="31">
-        <v>54004804001</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="F37" t="s">
+        <v>507</v>
+      </c>
+      <c r="G37" s="17"/>
       <c r="H37" s="17">
-        <v>0.3</v>
-      </c>
-      <c r="I37" s="30">
-        <v>1800</v>
+        <v>0.7</v>
+      </c>
+      <c r="I37" s="17">
+        <v>4050</v>
       </c>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
-        <v>231</v>
-      </c>
-      <c r="B38" t="s">
-        <v>530</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="B38" s="17"/>
       <c r="C38" s="17" t="s">
-        <v>276</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>311</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="D38" s="17"/>
       <c r="E38" s="17" t="s">
-        <v>11</v>
+        <v>129</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>498</v>
+        <v>548</v>
       </c>
       <c r="G38" s="31">
-        <v>54003011001</v>
+        <v>54004804001</v>
       </c>
       <c r="H38" s="17">
-        <v>20.8</v>
+        <v>0.3</v>
       </c>
       <c r="I38" s="30">
-        <v>48328</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
-        <v>268</v>
+        <v>231</v>
       </c>
       <c r="B39" t="s">
-        <v>531</v>
+        <v>497</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>308</v>
-      </c>
-      <c r="D39" s="17"/>
+        <v>276</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>311</v>
+      </c>
       <c r="E39" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="F39" s="17" t="s">
-        <v>582</v>
-      </c>
-      <c r="G39" s="17">
-        <v>54003703001</v>
+        <v>11</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="G39" s="31">
+        <v>54003011001</v>
       </c>
       <c r="H39" s="17">
-        <v>0.52500000000000002</v>
+        <v>20.8</v>
       </c>
       <c r="I39" s="30">
-        <v>2892</v>
+        <v>48328</v>
       </c>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B40" t="s">
-        <v>532</v>
+        <v>498</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="D40" s="17"/>
       <c r="E40" s="17" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>570</v>
-      </c>
-      <c r="G40" s="31">
-        <v>54003203001</v>
+        <v>549</v>
+      </c>
+      <c r="G40" s="17">
+        <v>54003703001</v>
       </c>
       <c r="H40" s="17">
-        <v>1.8</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="I40" s="30">
-        <v>3255</v>
+        <v>2892</v>
       </c>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
-        <v>270</v>
-      </c>
-      <c r="B41" s="17"/>
+        <v>269</v>
+      </c>
+      <c r="B41" t="s">
+        <v>499</v>
+      </c>
       <c r="C41" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D41" s="17"/>
       <c r="E41" s="17" t="s">
-        <v>122</v>
+        <v>15</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>571</v>
+        <v>537</v>
       </c>
       <c r="G41" s="31">
-        <v>54000509001</v>
+        <v>54003203001</v>
       </c>
       <c r="H41" s="17">
-        <v>4</v>
+        <v>1.8</v>
       </c>
       <c r="I41" s="30">
-        <v>20411</v>
+        <v>3255</v>
       </c>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>271</v>
-      </c>
-      <c r="B42" t="s">
-        <v>533</v>
-      </c>
+        <v>270</v>
+      </c>
+      <c r="B42" s="17"/>
       <c r="C42" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D42" s="17"/>
       <c r="E42" s="17" t="s">
-        <v>9</v>
+        <v>122</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>499</v>
-      </c>
-      <c r="G42" s="17">
-        <v>54002102001</v>
+        <v>538</v>
+      </c>
+      <c r="G42" s="31">
+        <v>54000509001</v>
       </c>
       <c r="H42" s="17">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="I42" s="30">
-        <v>10364</v>
+        <v>20411</v>
       </c>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B43" t="s">
-        <v>534</v>
+        <v>500</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D43" s="17"/>
       <c r="E43" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>500</v>
-      </c>
-      <c r="G43" s="31">
-        <v>54000901001</v>
+        <v>9</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>466</v>
+      </c>
+      <c r="G43" s="17">
+        <v>54002102001</v>
       </c>
       <c r="H43" s="17">
-        <v>0.2</v>
+        <v>2.5</v>
       </c>
       <c r="I43" s="30">
-        <v>564</v>
+        <v>10364</v>
       </c>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B44" t="s">
-        <v>535</v>
+        <v>501</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="D44" s="17"/>
       <c r="E44" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="G44" s="31">
+        <v>54000901001</v>
+      </c>
+      <c r="H44" s="17">
+        <v>0.2</v>
+      </c>
+      <c r="I44" s="30">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A45" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="B45" t="s">
+        <v>502</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>304</v>
+      </c>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F44" s="4" t="s">
-        <v>501</v>
-      </c>
-      <c r="G44" s="31">
+      <c r="F45" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="G45" s="31">
         <v>54003508001</v>
       </c>
-      <c r="H44" s="17">
+      <c r="H45" s="17">
         <v>10</v>
       </c>
-      <c r="I44" s="30">
+      <c r="I45" s="30">
         <v>33782</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
-        <v>584</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>569</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>479</v>
-      </c>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4" t="s">
+    <row r="46" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>536</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="F45" s="31" t="s">
-        <v>502</v>
-      </c>
-      <c r="G45" s="31">
+      <c r="F46" s="31" t="s">
+        <v>469</v>
+      </c>
+      <c r="G46" s="31">
         <v>54001022001</v>
       </c>
-      <c r="H45" s="4">
+      <c r="H46" s="4">
         <v>0.75</v>
       </c>
-      <c r="I45" s="19">
+      <c r="I46" s="19">
         <v>2626</v>
-      </c>
-    </row>
-    <row r="46" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="17" t="s">
-        <v>274</v>
-      </c>
-      <c r="B46" s="17"/>
-      <c r="C46" s="17" t="s">
-        <v>305</v>
-      </c>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="F46" s="17"/>
-      <c r="G46" s="31">
-        <v>54002422001</v>
-      </c>
-      <c r="H46" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="I46" s="30">
-        <v>2742</v>
       </c>
       <c r="J46" s="28"/>
       <c r="K46" s="2"/>
@@ -8623,30 +8616,26 @@
       <c r="W46"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="50" t="s">
-        <v>632</v>
-      </c>
-      <c r="B47" s="51" t="s">
-        <v>633</v>
-      </c>
-      <c r="C47" s="50" t="s">
-        <v>619</v>
-      </c>
-      <c r="D47" s="50" t="s">
-        <v>634</v>
-      </c>
-      <c r="E47" s="50" t="s">
-        <v>159</v>
-      </c>
-      <c r="F47" s="50" t="s">
-        <v>635</v>
-      </c>
-      <c r="G47" s="50"/>
-      <c r="H47" s="50">
-        <v>0.3</v>
-      </c>
-      <c r="I47" s="52">
-        <v>3500</v>
+      <c r="A47" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17" t="s">
+        <v>305</v>
+      </c>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F47" s="17"/>
+      <c r="G47" s="31">
+        <v>54002422001</v>
+      </c>
+      <c r="H47" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="I47" s="30">
+        <v>2742</v>
       </c>
       <c r="J47" s="51"/>
       <c r="K47" s="51"/>
@@ -8666,9 +8655,35 @@
       <c r="Y47" s="51"/>
       <c r="Z47" s="51"/>
     </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A48" s="17" t="s">
+        <v>621</v>
+      </c>
+      <c r="B48" t="s">
+        <v>624</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="D48" t="s">
+        <v>622</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="G48" s="31">
+        <v>54001601001</v>
+      </c>
+      <c r="H48" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I48" s="30">
+        <v>3510</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I46">
-    <sortCondition ref="A2:A46"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I47">
+    <sortCondition ref="A2:A47"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8679,7 +8694,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8698,7 +8713,7 @@
         <v>431</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>503</v>
+        <v>470</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>239</v>
@@ -8711,951 +8726,887 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>317</v>
-      </c>
+      <c r="A2" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="4"/>
       <c r="C2" s="17">
-        <v>54061</v>
+        <v>54001</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>11</v>
+        <v>123</v>
       </c>
       <c r="E2" s="18">
-        <v>105612</v>
+        <v>16633</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>318</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="B3" s="4"/>
       <c r="C3" s="17">
-        <v>54039</v>
+        <v>54003</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="20">
-        <v>183279</v>
+        <v>193</v>
+      </c>
+      <c r="E3" s="18">
+        <v>126069</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="C4" s="17">
-        <v>54069</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="18">
-        <v>41447</v>
+      <c r="A4" s="57" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" s="57" t="s">
+        <v>333</v>
+      </c>
+      <c r="C4" s="58">
+        <v>54005</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="E4" s="59">
+        <v>21809</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>320</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="B5" s="4"/>
       <c r="C5" s="17">
-        <v>54037</v>
+        <v>54007</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>7</v>
+        <v>194</v>
       </c>
       <c r="E5" s="18">
-        <v>57146</v>
+        <v>12247</v>
       </c>
       <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="C6" s="17">
-        <v>54055</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="18">
-        <v>58758</v>
+      <c r="A6" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="57" t="s">
+        <v>335</v>
+      </c>
+      <c r="C6" s="58">
+        <v>54009</v>
+      </c>
+      <c r="D6" s="58" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="59">
+        <v>21939</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>322</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="B7" s="4"/>
       <c r="C7" s="17">
-        <v>54041</v>
+        <v>54011</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="18">
-        <v>16166</v>
+        <v>157</v>
+      </c>
+      <c r="E7" s="20">
+        <v>96319</v>
       </c>
       <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>323</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="B8" s="4"/>
       <c r="C8" s="17">
-        <v>54057</v>
+        <v>54013</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>13</v>
+        <v>195</v>
       </c>
       <c r="E8" s="18">
-        <v>26868</v>
+        <v>6176</v>
       </c>
       <c r="F8" s="21"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>324</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="B9" s="4"/>
       <c r="C9" s="17">
-        <v>54051</v>
+        <v>54015</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>5</v>
+        <v>196</v>
       </c>
       <c r="E9" s="18">
-        <v>30531</v>
+        <v>7892</v>
       </c>
       <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="C10" s="17">
-        <v>54065</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="18">
-        <v>17884</v>
+      <c r="A10" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="57" t="s">
+        <v>328</v>
+      </c>
+      <c r="C10" s="58">
+        <v>54017</v>
+      </c>
+      <c r="D10" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="59">
+        <v>8448</v>
       </c>
       <c r="F10" s="21"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="C11" s="17">
-        <v>54077</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" s="18">
-        <v>33432</v>
+      <c r="A11" s="58" t="s">
+        <v>197</v>
+      </c>
+      <c r="B11" s="57" t="s">
+        <v>432</v>
+      </c>
+      <c r="C11" s="58">
+        <v>54019</v>
+      </c>
+      <c r="D11" s="58" t="s">
+        <v>197</v>
+      </c>
+      <c r="E11" s="59">
+        <v>39927</v>
       </c>
       <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>327</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="B12" s="4"/>
       <c r="C12" s="17">
-        <v>54107</v>
+        <v>54021</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>54</v>
+        <v>198</v>
       </c>
       <c r="E12" s="18">
-        <v>83518</v>
+        <v>7377</v>
       </c>
       <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="C13" s="17">
-        <v>54017</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="18">
-        <v>8448</v>
+      <c r="A13" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="57"/>
+      <c r="C13" s="58">
+        <v>54023</v>
+      </c>
+      <c r="D13" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="59">
+        <v>11616</v>
       </c>
       <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>329</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="B14" s="4"/>
       <c r="C14" s="17">
-        <v>54049</v>
+        <v>54025</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>89</v>
+        <v>199</v>
       </c>
       <c r="E14" s="18">
-        <v>56072</v>
+        <v>32608</v>
       </c>
       <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="17">
+        <v>54027</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="E15" s="18">
+        <v>23302</v>
+      </c>
+      <c r="F15" s="21"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="58" t="s">
+        <v>201</v>
+      </c>
+      <c r="B16" s="57"/>
+      <c r="C16" s="58">
+        <v>54029</v>
+      </c>
+      <c r="D16" s="58" t="s">
+        <v>201</v>
+      </c>
+      <c r="E16" s="59">
+        <v>28656</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="58" t="s">
+        <v>202</v>
+      </c>
+      <c r="B17" s="57" t="s">
+        <v>433</v>
+      </c>
+      <c r="C17" s="58">
+        <v>54031</v>
+      </c>
+      <c r="D17" s="58" t="s">
+        <v>202</v>
+      </c>
+      <c r="E17" s="59">
+        <v>14160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B18" s="57" t="s">
         <v>330</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C18" s="58">
         <v>54033</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D18" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E18" s="59">
         <v>67256</v>
-      </c>
-      <c r="F15" s="21"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="C16" s="17">
-        <v>54091</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E16" s="18">
-        <v>16695</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="C17" s="17">
-        <v>54073</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="18">
-        <v>7482</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="C18" s="17">
-        <v>54005</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="E18" s="18">
-        <v>21809</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>334</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="B19" s="4"/>
       <c r="C19" s="17">
-        <v>54083</v>
+        <v>54035</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="E19" s="18">
-        <v>28695</v>
+        <v>27738</v>
       </c>
       <c r="F19" s="19"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="C20" s="17">
-        <v>54009</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="E20" s="18">
-        <v>21939</v>
+      <c r="A20" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="57" t="s">
+        <v>320</v>
+      </c>
+      <c r="C20" s="58">
+        <v>54037</v>
+      </c>
+      <c r="D20" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="59">
+        <v>57146</v>
       </c>
       <c r="F20" s="22"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="C21" s="17">
-        <v>54053</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="E21" s="18">
-        <v>26700</v>
+      <c r="A21" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="57" t="s">
+        <v>318</v>
+      </c>
+      <c r="C21" s="58">
+        <v>54039</v>
+      </c>
+      <c r="D21" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="60">
+        <v>183279</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>432</v>
-      </c>
-      <c r="C22" s="17">
-        <v>54001</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="E22" s="18">
-        <v>16633</v>
+      <c r="A22" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="57" t="s">
+        <v>322</v>
+      </c>
+      <c r="C22" s="58">
+        <v>54041</v>
+      </c>
+      <c r="D22" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="59">
+        <v>16166</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>433</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="B23" s="4"/>
       <c r="C23" s="17">
-        <v>54003</v>
+        <v>54043</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="E23" s="18">
-        <v>126069</v>
+        <v>20126</v>
       </c>
       <c r="F23" s="21"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>434</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="B24" s="4"/>
       <c r="C24" s="17">
-        <v>54007</v>
+        <v>54045</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="E24" s="18">
-        <v>12247</v>
+        <v>31909</v>
       </c>
       <c r="F24" s="21"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="C25" s="17">
-        <v>54011</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="E25" s="20">
-        <v>96319</v>
+      <c r="A25" s="57" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="57" t="s">
+        <v>329</v>
+      </c>
+      <c r="C25" s="58">
+        <v>54049</v>
+      </c>
+      <c r="D25" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="59">
+        <v>56072</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="C26" s="17">
-        <v>54013</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="E26" s="18">
-        <v>6176</v>
+      <c r="A26" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="57" t="s">
+        <v>324</v>
+      </c>
+      <c r="C26" s="58">
+        <v>54051</v>
+      </c>
+      <c r="D26" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="59">
+        <v>30531</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>437</v>
-      </c>
-      <c r="C27" s="17">
-        <v>54015</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="E27" s="18">
-        <v>7892</v>
+      <c r="A27" s="57" t="s">
+        <v>190</v>
+      </c>
+      <c r="B27" s="57" t="s">
+        <v>336</v>
+      </c>
+      <c r="C27" s="58">
+        <v>54053</v>
+      </c>
+      <c r="D27" s="58" t="s">
+        <v>190</v>
+      </c>
+      <c r="E27" s="59">
+        <v>26700</v>
       </c>
       <c r="F27" s="19"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>438</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="B28" s="4"/>
       <c r="C28" s="17">
-        <v>54019</v>
+        <v>54047</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="E28" s="18">
-        <v>39927</v>
+        <v>18363</v>
       </c>
       <c r="F28" s="22"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>439</v>
-      </c>
-      <c r="C29" s="17">
-        <v>54021</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="E29" s="18">
-        <v>7377</v>
+      <c r="A29" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="57" t="s">
+        <v>321</v>
+      </c>
+      <c r="C29" s="58">
+        <v>54055</v>
+      </c>
+      <c r="D29" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="59">
+        <v>58758</v>
       </c>
       <c r="F29" s="22"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>440</v>
-      </c>
-      <c r="C30" s="17">
-        <v>54023</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E30" s="18">
-        <v>11616</v>
+      <c r="A30" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="57" t="s">
+        <v>323</v>
+      </c>
+      <c r="C30" s="58">
+        <v>54057</v>
+      </c>
+      <c r="D30" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="59">
+        <v>26868</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>441</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="B31" s="4"/>
       <c r="C31" s="17">
-        <v>54025</v>
+        <v>54059</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="E31" s="18">
-        <v>32608</v>
+        <v>23005</v>
       </c>
       <c r="F31" s="22"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>442</v>
-      </c>
-      <c r="C32" s="17">
-        <v>54027</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="E32" s="18">
-        <v>23302</v>
+      <c r="A32" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="57" t="s">
+        <v>317</v>
+      </c>
+      <c r="C32" s="58">
+        <v>54061</v>
+      </c>
+      <c r="D32" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="59">
+        <v>105612</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>443</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="B33" s="4"/>
       <c r="C33" s="17">
-        <v>54029</v>
+        <v>54063</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="E33" s="18">
-        <v>28656</v>
+        <v>12332</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>444</v>
-      </c>
-      <c r="C34" s="17">
-        <v>54031</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="E34" s="18">
-        <v>14160</v>
+      <c r="A34" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="57" t="s">
+        <v>325</v>
+      </c>
+      <c r="C34" s="58">
+        <v>54065</v>
+      </c>
+      <c r="D34" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="59">
+        <v>17884</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>445</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="B35" s="4"/>
       <c r="C35" s="17">
-        <v>54035</v>
+        <v>54067</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="E35" s="18">
-        <v>27738</v>
+        <v>24300</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="C36" s="17">
-        <v>54043</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="E36" s="18">
-        <v>20126</v>
+      <c r="A36" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="57" t="s">
+        <v>319</v>
+      </c>
+      <c r="C36" s="58">
+        <v>54069</v>
+      </c>
+      <c r="D36" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="59">
+        <v>41447</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>447</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="B37" s="4"/>
       <c r="C37" s="17">
-        <v>54045</v>
+        <v>54071</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="E37" s="18">
-        <v>31909</v>
+        <v>6142</v>
       </c>
       <c r="F37" s="19"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>448</v>
-      </c>
-      <c r="C38" s="17">
-        <v>54047</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="E38" s="18">
-        <v>18363</v>
+      <c r="A38" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="57" t="s">
+        <v>332</v>
+      </c>
+      <c r="C38" s="58">
+        <v>54073</v>
+      </c>
+      <c r="D38" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" s="59">
+        <v>7482</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>449</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="B39" s="4"/>
       <c r="C39" s="17">
-        <v>54059</v>
+        <v>54075</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="E39" s="18">
-        <v>23005</v>
+        <v>7841</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>450</v>
-      </c>
-      <c r="C40" s="17">
-        <v>54063</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="E40" s="18">
-        <v>12332</v>
+      <c r="A40" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="57" t="s">
+        <v>326</v>
+      </c>
+      <c r="C40" s="58">
+        <v>54077</v>
+      </c>
+      <c r="D40" s="58" t="s">
+        <v>63</v>
+      </c>
+      <c r="E40" s="59">
+        <v>33432</v>
       </c>
       <c r="F40" s="19"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
-        <v>209</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>451</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="B41" s="4"/>
       <c r="C41" s="17">
-        <v>54067</v>
+        <v>54079</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>209</v>
-      </c>
-      <c r="E41" s="18">
-        <v>24300</v>
+        <v>159</v>
+      </c>
+      <c r="E41" s="20">
+        <v>55486</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>452</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="B42" s="4"/>
       <c r="C42" s="17">
-        <v>54071</v>
+        <v>54081</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E42" s="18">
-        <v>6142</v>
+        <v>73771</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>453</v>
-      </c>
-      <c r="C43" s="17">
-        <v>54075</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="E43" s="18">
-        <v>7841</v>
+      <c r="A43" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="B43" s="57" t="s">
+        <v>334</v>
+      </c>
+      <c r="C43" s="58">
+        <v>54083</v>
+      </c>
+      <c r="D43" s="58" t="s">
+        <v>121</v>
+      </c>
+      <c r="E43" s="59">
+        <v>28695</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>454</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="B44" s="4"/>
       <c r="C44" s="17">
-        <v>54079</v>
+        <v>54085</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="E44" s="20">
-        <v>55486</v>
+        <v>213</v>
+      </c>
+      <c r="E44" s="18">
+        <v>8383</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>455</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="B45" s="4"/>
       <c r="C45" s="17">
-        <v>54081</v>
+        <v>54087</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E45" s="18">
-        <v>73771</v>
+        <v>13898</v>
       </c>
       <c r="F45" s="19"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>456</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="B46" s="4"/>
       <c r="C46" s="17">
-        <v>54085</v>
+        <v>54089</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E46" s="18">
-        <v>8383</v>
+        <v>11908</v>
       </c>
       <c r="F46" s="19"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>457</v>
-      </c>
-      <c r="C47" s="17">
-        <v>54087</v>
-      </c>
-      <c r="D47" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="E47" s="18">
-        <v>13898</v>
+      <c r="A47" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="B47" s="57" t="s">
+        <v>331</v>
+      </c>
+      <c r="C47" s="58">
+        <v>54091</v>
+      </c>
+      <c r="D47" s="58" t="s">
+        <v>100</v>
+      </c>
+      <c r="E47" s="59">
+        <v>16695</v>
       </c>
       <c r="F47" s="19"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>458</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="B48" s="4"/>
       <c r="C48" s="17">
-        <v>54089</v>
+        <v>54093</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E48" s="18">
-        <v>11908</v>
+        <v>6672</v>
       </c>
       <c r="F48" s="19"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>459</v>
-      </c>
-      <c r="C49" s="17">
-        <v>54093</v>
-      </c>
-      <c r="D49" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="E49" s="18">
-        <v>6672</v>
+      <c r="A49" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="B49" s="57"/>
+      <c r="C49" s="58">
+        <v>54095</v>
+      </c>
+      <c r="D49" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="E49" s="59">
+        <v>8811</v>
       </c>
       <c r="F49" s="19"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>460</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="B50" s="4"/>
       <c r="C50" s="17">
-        <v>54095</v>
+        <v>54097</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>129</v>
+        <v>217</v>
       </c>
       <c r="E50" s="18">
-        <v>8811</v>
+        <v>23791</v>
       </c>
       <c r="F50" s="19"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>461</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="B51" s="4"/>
       <c r="C51" s="17">
-        <v>54097</v>
+        <v>54099</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="E51" s="18">
-        <v>23791</v>
+        <v>164</v>
+      </c>
+      <c r="E51" s="20">
+        <v>42481</v>
       </c>
       <c r="F51" s="19"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>462</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="B52" s="4"/>
       <c r="C52" s="17">
-        <v>54099</v>
+        <v>54101</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E52" s="20">
-        <v>42481</v>
+        <v>218</v>
+      </c>
+      <c r="E52" s="18">
+        <v>8249</v>
       </c>
       <c r="F52" s="19"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>463</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="B53" s="4"/>
       <c r="C53" s="17">
-        <v>54101</v>
+        <v>54103</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E53" s="18">
-        <v>8249</v>
+        <v>14170</v>
       </c>
       <c r="F53" s="19"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>464</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="B54" s="4"/>
       <c r="C54" s="17">
-        <v>54103</v>
+        <v>54105</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E54" s="18">
-        <v>14170</v>
+        <v>5063</v>
       </c>
       <c r="F54" s="19"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>465</v>
-      </c>
-      <c r="C55" s="17">
-        <v>54105</v>
-      </c>
-      <c r="D55" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="E55" s="18">
-        <v>5063</v>
+      <c r="A55" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" s="57" t="s">
+        <v>327</v>
+      </c>
+      <c r="C55" s="58">
+        <v>54107</v>
+      </c>
+      <c r="D55" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="E55" s="59">
+        <v>83518</v>
       </c>
       <c r="F55" s="19"/>
     </row>
@@ -9663,9 +9614,7 @@
       <c r="A56" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>466</v>
-      </c>
+      <c r="B56" s="4"/>
       <c r="C56" s="17">
         <v>54109</v>
       </c>
@@ -9698,8 +9647,8 @@
       <c r="F62" s="22"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:E56">
-    <sortCondition ref="D2:D56"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E56">
+    <sortCondition ref="A2:A56"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9709,7 +9658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274C28A9-51BA-1349-BC2C-74CFA9B6CA14}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
@@ -9766,7 +9715,7 @@
     </row>
     <row r="3" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
-        <v>585</v>
+        <v>552</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>409</v>
@@ -9786,10 +9735,10 @@
     </row>
     <row r="4" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>586</v>
+        <v>553</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>601</v>
+        <v>568</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>417</v>
@@ -9818,7 +9767,7 @@
     </row>
     <row r="6" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
-        <v>587</v>
+        <v>554</v>
       </c>
       <c r="B6" s="25" t="s">
         <v>399</v>
@@ -9839,7 +9788,7 @@
     </row>
     <row r="7" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="s">
-        <v>588</v>
+        <v>555</v>
       </c>
       <c r="B7" s="25" t="s">
         <v>400</v>
@@ -9859,10 +9808,10 @@
     </row>
     <row r="8" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
-        <v>589</v>
+        <v>556</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>598</v>
+        <v>565</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>416</v>
@@ -9916,10 +9865,10 @@
     </row>
     <row r="11" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="43" t="s">
-        <v>590</v>
+        <v>557</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>602</v>
+        <v>569</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>417</v>
@@ -9928,12 +9877,12 @@
         <v>382</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>607</v>
+        <v>574</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="43" t="s">
-        <v>599</v>
+        <v>566</v>
       </c>
       <c r="B12" s="25" t="s">
         <v>395</v>
@@ -9953,7 +9902,7 @@
     </row>
     <row r="13" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="43" t="s">
-        <v>600</v>
+        <v>567</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>398</v>
@@ -9974,10 +9923,10 @@
     </row>
     <row r="14" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="43" t="s">
-        <v>644</v>
+        <v>611</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>651</v>
+        <v>618</v>
       </c>
       <c r="C14" s="25" t="s">
         <v>416</v>
@@ -9994,7 +9943,7 @@
     </row>
     <row r="15" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="43" t="s">
-        <v>641</v>
+        <v>608</v>
       </c>
       <c r="B15" s="25" t="s">
         <v>412</v>
@@ -10014,7 +9963,7 @@
     </row>
     <row r="16" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="43" t="s">
-        <v>591</v>
+        <v>558</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>403</v>
@@ -10034,7 +9983,7 @@
     </row>
     <row r="17" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="43" t="s">
-        <v>592</v>
+        <v>559</v>
       </c>
       <c r="B17" s="25" t="s">
         <v>407</v>
@@ -10055,7 +10004,7 @@
     </row>
     <row r="18" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="43" t="s">
-        <v>593</v>
+        <v>560</v>
       </c>
       <c r="B18" s="25" t="s">
         <v>391</v>
@@ -10095,10 +10044,10 @@
     </row>
     <row r="20" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
-        <v>594</v>
+        <v>561</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>603</v>
+        <v>570</v>
       </c>
       <c r="C20" s="25" t="s">
         <v>417</v>
@@ -10112,10 +10061,10 @@
     </row>
     <row r="21" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="43" t="s">
-        <v>595</v>
+        <v>562</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>606</v>
+        <v>573</v>
       </c>
       <c r="C21" s="25" t="s">
         <v>417</v>
@@ -10129,10 +10078,10 @@
     </row>
     <row r="22" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="43" t="s">
-        <v>596</v>
+        <v>563</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>604</v>
+        <v>571</v>
       </c>
       <c r="C22" s="25" t="s">
         <v>417</v>
@@ -10146,10 +10095,10 @@
     </row>
     <row r="23" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="43" t="s">
-        <v>597</v>
+        <v>564</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>605</v>
+        <v>572</v>
       </c>
       <c r="C23" s="25" t="s">
         <v>417</v>
@@ -10285,23 +10234,23 @@
         <v>374</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>614</v>
+        <v>581</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>586</v>
+        <v>553</v>
       </c>
       <c r="B2" s="44" t="s">
-        <v>609</v>
+        <v>576</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>636</v>
+        <v>603</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>612</v>
+        <v>579</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -10317,31 +10266,31 @@
         <v>386</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>637</v>
+        <v>604</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>590</v>
+        <v>557</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>608</v>
+        <v>575</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="s">
-        <v>599</v>
+        <v>566</v>
       </c>
       <c r="B7" s="44" t="s">
-        <v>610</v>
+        <v>577</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="44" t="s">
-        <v>600</v>
+        <v>567</v>
       </c>
       <c r="B8" s="44" t="s">
-        <v>613</v>
+        <v>580</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -10349,7 +10298,7 @@
         <v>393</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>638</v>
+        <v>605</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -10357,7 +10306,7 @@
         <v>393</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>639</v>
+        <v>606</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -10365,12 +10314,12 @@
         <v>393</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>640</v>
+        <v>607</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
-        <v>593</v>
+        <v>560</v>
       </c>
       <c r="B12" s="25" t="s">
         <v>323</v>
@@ -10378,42 +10327,42 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
-        <v>641</v>
+        <v>608</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>642</v>
+        <v>609</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="53" t="s">
-        <v>592</v>
+        <v>559</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>643</v>
+        <v>610</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="54" t="s">
-        <v>588</v>
+        <v>555</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>643</v>
+        <v>610</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="54" t="s">
-        <v>589</v>
+        <v>556</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>643</v>
+        <v>610</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="53" t="s">
-        <v>644</v>
+        <v>611</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>611</v>
+        <v>578</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -10452,10 +10401,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="55" t="s">
-        <v>645</v>
+        <v>612</v>
       </c>
       <c r="B1" s="55" t="s">
-        <v>646</v>
+        <v>613</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -10463,7 +10412,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="56" t="s">
-        <v>647</v>
+        <v>614</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="51" x14ac:dyDescent="0.2">
@@ -10471,7 +10420,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>648</v>
+        <v>615</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -10491,7 +10440,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="56" t="s">
-        <v>649</v>
+        <v>616</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="51" x14ac:dyDescent="0.2">
@@ -10499,7 +10448,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="56" t="s">
-        <v>650</v>
+        <v>617</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Activated the Weston facility.
</commit_message>
<xml_diff>
--- a/dashboard/data/watchdb.all_tables.xlsx
+++ b/dashboard/data/watchdb.all_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB8D82C-FF40-BB4C-B0C5-3D32D8DF0B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E2E62F-3CD1-4E48-AF7D-0238DD5C037D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -2591,11 +2591,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0856F7A-D0C0-3942-9027-9FB2F3C2C3E0}">
   <dimension ref="A1:T82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Q33" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="O36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q83" sqref="Q83"/>
+      <selection pane="bottomRight" activeCell="T70" sqref="T70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6649,8 +6649,8 @@
       <c r="C70" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="D70" s="40" t="s">
-        <v>60</v>
+      <c r="D70" s="4" t="s">
+        <v>103</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>83</v>
@@ -7373,7 +7373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7706D3C3-8C4A-6E4A-999A-41BCCB2FAC67}">
   <dimension ref="A1:Z48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+    <sheetView zoomScale="133" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>

</xml_diff>

<commit_message>
Data update (partial). Latest sample from West Union excluded for abnormal high SC2; currently bring confirmed.
</commit_message>
<xml_diff>
--- a/dashboard/data/watchdb.all_tables.xlsx
+++ b/dashboard/data/watchdb.all_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/dashboard/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1CE0FE-9A0A-5E48-9BB9-3B63DF604BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370D7818-8CB1-0B49-BB60-62C23B6BA3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16500" yWindow="840" windowWidth="30240" windowHeight="18880" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="627">
   <si>
     <t>CharlestonWWTP-01</t>
   </si>
@@ -1921,6 +1921,9 @@
   </si>
   <si>
     <t>WV0020150</t>
+  </si>
+  <si>
+    <t>L01</t>
   </si>
 </sst>
 </file>
@@ -2592,10 +2595,10 @@
   <dimension ref="A1:T82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D65" sqref="D65"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3090,7 +3093,7 @@
         <v>52</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>525</v>
+        <v>626</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>351</v>

</xml_diff>

<commit_message>
Data update. Also added current date to the UI for easier ref.
</commit_message>
<xml_diff>
--- a/dashboard/data/watchdb.all_tables.xlsx
+++ b/dashboard/data/watchdb.all_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370D7818-8CB1-0B49-BB60-62C23B6BA3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8099E5-1D11-C34D-811F-5AEA3BF7A012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="55020" yWindow="4560" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="628">
   <si>
     <t>CharlestonWWTP-01</t>
   </si>
@@ -1924,6 +1924,9 @@
   </si>
   <si>
     <t>L01</t>
+  </si>
+  <si>
+    <t>Host</t>
   </si>
 </sst>
 </file>
@@ -2594,11 +2597,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0856F7A-D0C0-3942-9027-9FB2F3C2C3E0}">
   <dimension ref="A1:T82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7378,7 +7381,7 @@
   <dimension ref="A1:Z48"/>
   <sheetViews>
     <sheetView zoomScale="133" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
@@ -9668,9 +9671,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274C28A9-51BA-1349-BC2C-74CFA9B6CA14}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10138,6 +10141,23 @@
       </c>
       <c r="F24" s="25" t="s">
         <v>394</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A25" s="42" t="s">
+        <v>603</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>603</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>627</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>627</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Rearranged COVID tab to emphasize key alert levels and alert level info.
</commit_message>
<xml_diff>
--- a/dashboard/data/watchdb.all_tables.xlsx
+++ b/dashboard/data/watchdb.all_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8099E5-1D11-C34D-811F-5AEA3BF7A012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD31BBB0-D03C-634A-AB88-78C828B3F142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="55020" yWindow="4560" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -2597,11 +2597,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0856F7A-D0C0-3942-9027-9FB2F3C2C3E0}">
   <dimension ref="A1:T82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q29" sqref="Q29"/>
+      <selection pane="bottomRight" activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4300,7 +4300,7 @@
         <v>3</v>
       </c>
       <c r="L29" s="37">
-        <v>50000</v>
+        <v>33782</v>
       </c>
       <c r="M29" s="37" t="s">
         <v>338</v>
@@ -7380,9 +7380,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7706D3C3-8C4A-6E4A-999A-41BCCB2FAC67}">
   <dimension ref="A1:Z48"/>
   <sheetViews>
-    <sheetView zoomScale="133" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
+    <sheetView topLeftCell="B1" zoomScale="133" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8707,7 +8707,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9671,7 +9671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274C28A9-51BA-1349-BC2C-74CFA9B6CA14}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>

</xml_diff>